<commit_message>
PAE-448: Introduces Summary Log validation check for missing rows
</commit_message>
<xml_diff>
--- a/src/data/fixtures/uploads/reprocessor.xlsx
+++ b/src/data/fixtures/uploads/reprocessor.xlsx
@@ -188,9 +188,6 @@
     <t>__EPR_META_ACCREDITATION</t>
   </si>
   <si>
-    <t>68f6a147c117aec8a1ab7495</t>
-  </si>
-  <si>
     <t>__EPR_META_REGISTRATION</t>
   </si>
   <si>
@@ -681,6 +678,9 @@
   </si>
   <si>
     <t>Actual weight (100%)</t>
+  </si>
+  <si>
+    <t>Calc</t>
   </si>
   <si>
     <t>A W Jenkinson Woodwaste Ltd</t>
@@ -6818,14 +6818,12 @@
       <c r="C12" t="s" s="22">
         <v>11</v>
       </c>
-      <c r="D12" t="s" s="21">
+      <c r="D12" s="21"/>
+      <c r="E12" t="s" s="22">
         <v>12</v>
       </c>
-      <c r="E12" t="s" s="22">
+      <c r="F12" t="s" s="21">
         <v>13</v>
-      </c>
-      <c r="F12" t="s" s="21">
-        <v>14</v>
       </c>
       <c r="G12" s="23"/>
       <c r="H12" s="9"/>
@@ -7937,7 +7935,7 @@
       <c r="AB2" s="36"/>
       <c r="AC2" s="36"/>
       <c r="AD2" t="s" s="37">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AE2" s="38"/>
       <c r="AF2" s="38"/>
@@ -7950,7 +7948,7 @@
     <row r="3" ht="56.1" customHeight="1">
       <c r="A3" s="6"/>
       <c r="B3" t="s" s="40">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="41"/>
       <c r="D3" s="42"/>
@@ -7967,26 +7965,26 @@
       <c r="O3" s="9"/>
       <c r="P3" s="35"/>
       <c r="Q3" t="s" s="43">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R3" s="44"/>
       <c r="S3" s="45"/>
       <c r="T3" s="35"/>
       <c r="U3" t="s" s="46">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V3" s="35"/>
       <c r="W3" s="31"/>
       <c r="X3" s="36"/>
       <c r="Y3" t="s" s="43">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Z3" s="44"/>
       <c r="AA3" s="47"/>
       <c r="AB3" s="47"/>
       <c r="AC3" s="47"/>
       <c r="AD3" t="s" s="37">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AE3" s="48"/>
       <c r="AF3" s="48"/>
@@ -7999,13 +7997,13 @@
     <row r="4" ht="56.1" customHeight="1">
       <c r="A4" s="50"/>
       <c r="B4" t="s" s="51">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="53"/>
       <c r="E4" s="54"/>
       <c r="F4" t="s" s="55">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="56"/>
       <c r="H4" s="56"/>
@@ -8018,19 +8016,19 @@
       <c r="O4" s="9"/>
       <c r="P4" s="57"/>
       <c r="Q4" t="s" s="58">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R4" s="59"/>
       <c r="S4" s="60"/>
       <c r="T4" s="61"/>
       <c r="U4" t="s" s="46">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V4" s="35"/>
       <c r="W4" s="31"/>
       <c r="X4" s="62"/>
       <c r="Y4" t="s" s="63">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Z4" s="64"/>
       <c r="AA4" s="64"/>
@@ -8087,43 +8085,43 @@
     <row r="6" ht="96" customHeight="1">
       <c r="A6" s="71"/>
       <c r="B6" t="s" s="72">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s" s="73">
         <v>26</v>
       </c>
-      <c r="C6" t="s" s="73">
+      <c r="D6" t="s" s="73">
         <v>27</v>
       </c>
-      <c r="D6" t="s" s="73">
+      <c r="E6" t="s" s="73">
         <v>28</v>
       </c>
-      <c r="E6" t="s" s="73">
+      <c r="F6" t="s" s="73">
         <v>29</v>
       </c>
-      <c r="F6" t="s" s="73">
+      <c r="G6" t="s" s="73">
         <v>30</v>
       </c>
-      <c r="G6" t="s" s="73">
+      <c r="H6" t="s" s="73">
         <v>31</v>
       </c>
-      <c r="H6" t="s" s="73">
+      <c r="I6" t="s" s="73">
         <v>32</v>
       </c>
-      <c r="I6" t="s" s="73">
+      <c r="J6" t="s" s="73">
         <v>33</v>
       </c>
-      <c r="J6" t="s" s="73">
+      <c r="K6" t="s" s="73">
         <v>34</v>
       </c>
-      <c r="K6" t="s" s="73">
+      <c r="L6" t="s" s="73">
         <v>35</v>
       </c>
-      <c r="L6" t="s" s="73">
+      <c r="M6" t="s" s="73">
         <v>36</v>
       </c>
-      <c r="M6" t="s" s="73">
+      <c r="N6" t="s" s="73">
         <v>37</v>
-      </c>
-      <c r="N6" t="s" s="73">
-        <v>38</v>
       </c>
       <c r="O6" s="74">
         <v>1</v>
@@ -8132,22 +8130,22 @@
         <v>2</v>
       </c>
       <c r="Q6" t="s" s="76">
+        <v>38</v>
+      </c>
+      <c r="R6" t="s" s="76">
         <v>39</v>
       </c>
-      <c r="R6" t="s" s="76">
+      <c r="S6" t="s" s="76">
         <v>40</v>
       </c>
-      <c r="S6" t="s" s="76">
+      <c r="T6" t="s" s="76">
         <v>41</v>
       </c>
-      <c r="T6" t="s" s="76">
+      <c r="U6" t="s" s="77">
         <v>42</v>
       </c>
-      <c r="U6" t="s" s="77">
+      <c r="V6" t="s" s="76">
         <v>43</v>
-      </c>
-      <c r="V6" t="s" s="76">
-        <v>44</v>
       </c>
       <c r="W6" s="78">
         <v>3</v>
@@ -8156,22 +8154,22 @@
         <v>4</v>
       </c>
       <c r="Y6" t="s" s="73">
+        <v>44</v>
+      </c>
+      <c r="Z6" t="s" s="76">
         <v>45</v>
       </c>
-      <c r="Z6" t="s" s="76">
+      <c r="AA6" t="s" s="76">
         <v>46</v>
       </c>
-      <c r="AA6" t="s" s="76">
+      <c r="AB6" t="s" s="76">
         <v>47</v>
       </c>
-      <c r="AB6" t="s" s="76">
+      <c r="AC6" t="s" s="76">
         <v>48</v>
       </c>
-      <c r="AC6" t="s" s="76">
+      <c r="AD6" t="s" s="76">
         <v>49</v>
-      </c>
-      <c r="AD6" t="s" s="76">
-        <v>50</v>
       </c>
       <c r="AE6" s="80">
         <v>5</v>
@@ -8185,94 +8183,94 @@
     </row>
     <row r="7" ht="48.75" customHeight="1">
       <c r="A7" t="s" s="83">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s" s="84">
         <v>51</v>
       </c>
-      <c r="B7" t="s" s="84">
+      <c r="C7" t="s" s="84">
         <v>52</v>
       </c>
-      <c r="C7" t="s" s="84">
+      <c r="D7" t="s" s="84">
         <v>53</v>
       </c>
-      <c r="D7" t="s" s="84">
+      <c r="E7" t="s" s="84">
         <v>54</v>
       </c>
-      <c r="E7" t="s" s="84">
+      <c r="F7" t="s" s="84">
         <v>55</v>
       </c>
-      <c r="F7" t="s" s="84">
+      <c r="G7" t="s" s="84">
         <v>56</v>
       </c>
-      <c r="G7" t="s" s="84">
+      <c r="H7" t="s" s="84">
         <v>57</v>
       </c>
-      <c r="H7" t="s" s="84">
+      <c r="I7" t="s" s="84">
         <v>58</v>
       </c>
-      <c r="I7" t="s" s="84">
+      <c r="J7" t="s" s="84">
         <v>59</v>
       </c>
-      <c r="J7" t="s" s="84">
+      <c r="K7" t="s" s="84">
         <v>60</v>
       </c>
-      <c r="K7" t="s" s="84">
+      <c r="L7" t="s" s="84">
         <v>61</v>
       </c>
-      <c r="L7" t="s" s="84">
+      <c r="M7" t="s" s="84">
         <v>62</v>
       </c>
-      <c r="M7" t="s" s="84">
+      <c r="N7" t="s" s="84">
         <v>63</v>
       </c>
-      <c r="N7" t="s" s="84">
+      <c r="O7" t="s" s="85">
         <v>64</v>
       </c>
-      <c r="O7" t="s" s="85">
+      <c r="P7" t="s" s="86">
         <v>65</v>
       </c>
-      <c r="P7" t="s" s="86">
+      <c r="Q7" t="s" s="87">
         <v>66</v>
       </c>
-      <c r="Q7" t="s" s="87">
+      <c r="R7" t="s" s="87">
         <v>67</v>
       </c>
-      <c r="R7" t="s" s="87">
+      <c r="S7" t="s" s="87">
         <v>68</v>
       </c>
-      <c r="S7" t="s" s="87">
+      <c r="T7" t="s" s="87">
         <v>69</v>
       </c>
-      <c r="T7" t="s" s="87">
+      <c r="U7" t="s" s="88">
         <v>70</v>
       </c>
-      <c r="U7" t="s" s="88">
+      <c r="V7" t="s" s="87">
         <v>71</v>
       </c>
-      <c r="V7" t="s" s="87">
+      <c r="W7" t="s" s="89">
+        <v>64</v>
+      </c>
+      <c r="X7" t="s" s="90">
         <v>72</v>
       </c>
-      <c r="W7" t="s" s="89">
-        <v>65</v>
-      </c>
-      <c r="X7" t="s" s="90">
+      <c r="Y7" t="s" s="91">
         <v>73</v>
       </c>
-      <c r="Y7" t="s" s="91">
+      <c r="Z7" t="s" s="87">
         <v>74</v>
       </c>
-      <c r="Z7" t="s" s="87">
+      <c r="AA7" t="s" s="87">
         <v>75</v>
       </c>
-      <c r="AA7" t="s" s="87">
+      <c r="AB7" t="s" s="87">
         <v>76</v>
       </c>
-      <c r="AB7" t="s" s="87">
+      <c r="AC7" t="s" s="87">
         <v>77</v>
       </c>
-      <c r="AC7" t="s" s="87">
+      <c r="AD7" t="s" s="87">
         <v>78</v>
-      </c>
-      <c r="AD7" t="s" s="87">
-        <v>79</v>
       </c>
       <c r="AE7" s="92"/>
       <c r="AF7" s="92"/>
@@ -8284,7 +8282,7 @@
     </row>
     <row r="8" ht="96" customHeight="1">
       <c r="A8" t="s" s="94">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="95" cm="1">
         <f t="array" ref="B8">IF(COUNTA(F8:G8)=0,"",9992+ROW())</f>
@@ -8294,10 +8292,10 @@
         <v>45805</v>
       </c>
       <c r="D8" t="s" s="97">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" t="s" s="97">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F8" s="98">
         <v>50</v>
@@ -8313,10 +8311,10 @@
         <v>30</v>
       </c>
       <c r="J8" t="s" s="97">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K8" t="s" s="97">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L8" s="98">
         <v>5</v>
@@ -8330,44 +8328,44 @@
       </c>
       <c r="O8" s="101"/>
       <c r="P8" t="s" s="102">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q8" t="s" s="97">
+        <v>82</v>
+      </c>
+      <c r="R8" t="s" s="97">
         <v>83</v>
       </c>
-      <c r="R8" t="s" s="97">
+      <c r="S8" t="s" s="97">
         <v>84</v>
       </c>
-      <c r="S8" t="s" s="97">
+      <c r="T8" t="s" s="103">
         <v>85</v>
-      </c>
-      <c r="T8" t="s" s="103">
-        <v>86</v>
       </c>
       <c r="U8" s="104">
         <v>1234567890</v>
       </c>
       <c r="V8" t="s" s="97">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="W8" s="105"/>
       <c r="X8" t="s" s="106">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Y8" t="s" s="97">
+        <v>87</v>
+      </c>
+      <c r="Z8" t="s" s="97">
         <v>88</v>
       </c>
-      <c r="Z8" t="s" s="97">
+      <c r="AA8" t="s" s="97">
         <v>89</v>
       </c>
-      <c r="AA8" t="s" s="97">
+      <c r="AB8" t="s" s="97">
         <v>90</v>
       </c>
-      <c r="AB8" t="s" s="97">
+      <c r="AC8" t="s" s="97">
         <v>91</v>
-      </c>
-      <c r="AC8" t="s" s="97">
-        <v>92</v>
       </c>
       <c r="AD8" s="107"/>
       <c r="AE8" s="108"/>
@@ -8388,10 +8386,10 @@
         <v>45870</v>
       </c>
       <c r="D9" t="s" s="84">
+        <v>92</v>
+      </c>
+      <c r="E9" t="s" s="84">
         <v>93</v>
-      </c>
-      <c r="E9" t="s" s="84">
-        <v>94</v>
       </c>
       <c r="F9" s="111">
         <v>10000</v>
@@ -8407,10 +8405,10 @@
         <v>4495</v>
       </c>
       <c r="J9" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K9" t="s" s="84">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L9" s="111">
         <v>21</v>
@@ -8425,42 +8423,42 @@
       <c r="O9" s="101"/>
       <c r="P9" s="57"/>
       <c r="Q9" t="s" s="84">
+        <v>95</v>
+      </c>
+      <c r="R9" t="s" s="84">
         <v>96</v>
       </c>
-      <c r="R9" t="s" s="84">
+      <c r="S9" t="s" s="84">
         <v>97</v>
       </c>
-      <c r="S9" t="s" s="84">
+      <c r="T9" t="s" s="114">
         <v>98</v>
       </c>
-      <c r="T9" t="s" s="114">
+      <c r="U9" t="s" s="115">
         <v>99</v>
       </c>
-      <c r="U9" t="s" s="115">
+      <c r="V9" t="s" s="84">
         <v>100</v>
-      </c>
-      <c r="V9" t="s" s="84">
-        <v>101</v>
       </c>
       <c r="W9" s="116"/>
       <c r="X9" s="62"/>
       <c r="Y9" t="s" s="84">
+        <v>101</v>
+      </c>
+      <c r="Z9" t="s" s="84">
         <v>102</v>
       </c>
-      <c r="Z9" t="s" s="84">
+      <c r="AA9" t="s" s="84">
         <v>103</v>
       </c>
-      <c r="AA9" t="s" s="84">
+      <c r="AB9" t="s" s="84">
         <v>104</v>
       </c>
-      <c r="AB9" t="s" s="84">
+      <c r="AC9" t="s" s="84">
         <v>105</v>
       </c>
-      <c r="AC9" t="s" s="84">
+      <c r="AD9" t="s" s="84">
         <v>106</v>
-      </c>
-      <c r="AD9" t="s" s="84">
-        <v>107</v>
       </c>
       <c r="AE9" s="117"/>
       <c r="AF9" s="48"/>
@@ -8480,10 +8478,10 @@
         <v>45905</v>
       </c>
       <c r="D10" t="s" s="84">
+        <v>107</v>
+      </c>
+      <c r="E10" t="s" s="84">
         <v>108</v>
-      </c>
-      <c r="E10" t="s" s="84">
-        <v>109</v>
       </c>
       <c r="F10" s="111">
         <v>3640</v>
@@ -8499,10 +8497,10 @@
         <v>1840</v>
       </c>
       <c r="J10" t="s" s="84">
+        <v>109</v>
+      </c>
+      <c r="K10" t="s" s="84">
         <v>110</v>
-      </c>
-      <c r="K10" t="s" s="84">
-        <v>111</v>
       </c>
       <c r="L10" s="111">
         <v>115</v>
@@ -8517,42 +8515,42 @@
       <c r="O10" s="101"/>
       <c r="P10" s="57"/>
       <c r="Q10" t="s" s="84">
+        <v>111</v>
+      </c>
+      <c r="R10" t="s" s="84">
         <v>112</v>
       </c>
-      <c r="R10" t="s" s="84">
+      <c r="S10" t="s" s="84">
         <v>113</v>
       </c>
-      <c r="S10" t="s" s="84">
+      <c r="T10" t="s" s="114">
         <v>114</v>
       </c>
-      <c r="T10" t="s" s="114">
+      <c r="U10" t="s" s="115">
         <v>115</v>
       </c>
-      <c r="U10" t="s" s="115">
+      <c r="V10" t="s" s="84">
         <v>116</v>
-      </c>
-      <c r="V10" t="s" s="84">
-        <v>117</v>
       </c>
       <c r="W10" s="116"/>
       <c r="X10" s="62"/>
       <c r="Y10" t="s" s="84">
+        <v>117</v>
+      </c>
+      <c r="Z10" t="s" s="84">
         <v>118</v>
       </c>
-      <c r="Z10" t="s" s="84">
+      <c r="AA10" t="s" s="84">
         <v>119</v>
       </c>
-      <c r="AA10" t="s" s="84">
+      <c r="AB10" t="s" s="84">
         <v>120</v>
       </c>
-      <c r="AB10" t="s" s="84">
+      <c r="AC10" t="s" s="84">
         <v>121</v>
       </c>
-      <c r="AC10" t="s" s="84">
+      <c r="AD10" t="s" s="84">
         <v>122</v>
-      </c>
-      <c r="AD10" t="s" s="84">
-        <v>123</v>
       </c>
       <c r="AE10" s="117"/>
       <c r="AF10" s="48"/>
@@ -8572,10 +8570,10 @@
         <v>45900</v>
       </c>
       <c r="D11" t="s" s="84">
+        <v>123</v>
+      </c>
+      <c r="E11" t="s" s="84">
         <v>124</v>
-      </c>
-      <c r="E11" t="s" s="84">
-        <v>125</v>
       </c>
       <c r="F11" s="111">
         <v>3615</v>
@@ -8591,10 +8589,10 @@
         <v>1930</v>
       </c>
       <c r="J11" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K11" t="s" s="84">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L11" s="111">
         <v>120</v>
@@ -8609,42 +8607,42 @@
       <c r="O11" s="101"/>
       <c r="P11" s="57"/>
       <c r="Q11" t="s" s="84">
+        <v>126</v>
+      </c>
+      <c r="R11" t="s" s="84">
         <v>127</v>
       </c>
-      <c r="R11" t="s" s="84">
+      <c r="S11" t="s" s="84">
         <v>128</v>
       </c>
-      <c r="S11" t="s" s="84">
+      <c r="T11" t="s" s="114">
         <v>129</v>
       </c>
-      <c r="T11" t="s" s="114">
+      <c r="U11" t="s" s="115">
         <v>130</v>
       </c>
-      <c r="U11" t="s" s="115">
+      <c r="V11" t="s" s="84">
         <v>131</v>
-      </c>
-      <c r="V11" t="s" s="84">
-        <v>132</v>
       </c>
       <c r="W11" s="116"/>
       <c r="X11" s="62"/>
       <c r="Y11" t="s" s="84">
+        <v>132</v>
+      </c>
+      <c r="Z11" t="s" s="84">
         <v>133</v>
       </c>
-      <c r="Z11" t="s" s="84">
+      <c r="AA11" t="s" s="84">
         <v>134</v>
       </c>
-      <c r="AA11" t="s" s="84">
+      <c r="AB11" t="s" s="84">
         <v>135</v>
       </c>
-      <c r="AB11" t="s" s="84">
+      <c r="AC11" t="s" s="84">
         <v>136</v>
       </c>
-      <c r="AC11" t="s" s="84">
+      <c r="AD11" t="s" s="84">
         <v>137</v>
-      </c>
-      <c r="AD11" t="s" s="84">
-        <v>138</v>
       </c>
       <c r="AE11" s="117"/>
       <c r="AF11" s="48"/>
@@ -8664,10 +8662,10 @@
         <v>45871</v>
       </c>
       <c r="D12" t="s" s="84">
+        <v>138</v>
+      </c>
+      <c r="E12" t="s" s="84">
         <v>139</v>
-      </c>
-      <c r="E12" t="s" s="84">
-        <v>140</v>
       </c>
       <c r="F12" s="111">
         <v>10050</v>
@@ -8683,10 +8681,10 @@
         <v>4385</v>
       </c>
       <c r="J12" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K12" t="s" s="84">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L12" s="111">
         <v>125</v>
@@ -8701,42 +8699,42 @@
       <c r="O12" s="101"/>
       <c r="P12" s="57"/>
       <c r="Q12" t="s" s="84">
+        <v>141</v>
+      </c>
+      <c r="R12" t="s" s="84">
         <v>142</v>
       </c>
-      <c r="R12" t="s" s="84">
+      <c r="S12" t="s" s="84">
         <v>143</v>
       </c>
-      <c r="S12" t="s" s="84">
+      <c r="T12" t="s" s="114">
         <v>144</v>
       </c>
-      <c r="T12" t="s" s="114">
+      <c r="U12" t="s" s="115">
+        <v>99</v>
+      </c>
+      <c r="V12" t="s" s="84">
         <v>145</v>
-      </c>
-      <c r="U12" t="s" s="115">
-        <v>100</v>
-      </c>
-      <c r="V12" t="s" s="84">
-        <v>146</v>
       </c>
       <c r="W12" s="116"/>
       <c r="X12" s="62"/>
       <c r="Y12" t="s" s="84">
+        <v>146</v>
+      </c>
+      <c r="Z12" t="s" s="84">
         <v>147</v>
       </c>
-      <c r="Z12" t="s" s="84">
+      <c r="AA12" t="s" s="84">
         <v>148</v>
       </c>
-      <c r="AA12" t="s" s="84">
+      <c r="AB12" t="s" s="84">
         <v>149</v>
       </c>
-      <c r="AB12" t="s" s="84">
+      <c r="AC12" t="s" s="84">
         <v>150</v>
       </c>
-      <c r="AC12" t="s" s="84">
-        <v>151</v>
-      </c>
       <c r="AD12" t="s" s="84">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AE12" s="117"/>
       <c r="AF12" s="48"/>
@@ -8756,10 +8754,10 @@
         <v>45905</v>
       </c>
       <c r="D13" t="s" s="84">
+        <v>107</v>
+      </c>
+      <c r="E13" t="s" s="84">
         <v>108</v>
-      </c>
-      <c r="E13" t="s" s="84">
-        <v>109</v>
       </c>
       <c r="F13" s="111">
         <v>3640</v>
@@ -8775,10 +8773,10 @@
         <v>1840</v>
       </c>
       <c r="J13" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K13" t="s" s="84">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L13" s="111">
         <v>23</v>
@@ -8786,9 +8784,8 @@
       <c r="M13" s="113">
         <v>0.95</v>
       </c>
-      <c r="N13" s="111" cm="1">
-        <f t="array" ref="N13">_xlfn.IFERROR((IF(IF(J13="Yes",((I13-(I13*0.15%))*M13),(I13*M13))=0,"",IF(J13="Yes",((I13-(I13*0.15%))*M13),(I13*M13)))-L13),"")</f>
-        <v>1722.378</v>
+      <c r="N13" t="s" s="84">
+        <v>152</v>
       </c>
       <c r="O13" s="101"/>
       <c r="P13" s="57"/>
@@ -8802,13 +8799,13 @@
         <v>155</v>
       </c>
       <c r="T13" t="s" s="114">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="U13" t="s" s="115">
         <v>156</v>
       </c>
       <c r="V13" t="s" s="84">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W13" s="116"/>
       <c r="X13" s="62"/>
@@ -8848,10 +8845,10 @@
         <v>45900</v>
       </c>
       <c r="D14" t="s" s="84">
+        <v>123</v>
+      </c>
+      <c r="E14" t="s" s="84">
         <v>124</v>
-      </c>
-      <c r="E14" t="s" s="84">
-        <v>125</v>
       </c>
       <c r="F14" s="111">
         <v>3615</v>
@@ -8867,10 +8864,10 @@
         <v>1930</v>
       </c>
       <c r="J14" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K14" t="s" s="84">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L14" s="111">
         <v>115</v>
@@ -8894,13 +8891,13 @@
         <v>165</v>
       </c>
       <c r="T14" t="s" s="114">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="U14" t="s" s="115">
         <v>166</v>
       </c>
       <c r="V14" t="s" s="84">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="W14" s="116"/>
       <c r="X14" s="62"/>
@@ -8959,10 +8956,10 @@
         <v>4275</v>
       </c>
       <c r="J15" t="s" s="84">
+        <v>109</v>
+      </c>
+      <c r="K15" t="s" s="84">
         <v>110</v>
-      </c>
-      <c r="K15" t="s" s="84">
-        <v>111</v>
       </c>
       <c r="L15" s="111">
         <v>120</v>
@@ -8977,7 +8974,7 @@
       <c r="O15" s="101"/>
       <c r="P15" s="57"/>
       <c r="Q15" t="s" s="84">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="R15" t="s" s="84">
         <v>175</v>
@@ -8986,13 +8983,13 @@
         <v>176</v>
       </c>
       <c r="T15" t="s" s="114">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="U15" t="s" s="115">
         <v>177</v>
       </c>
       <c r="V15" t="s" s="84">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W15" s="116"/>
       <c r="X15" s="62"/>
@@ -9032,10 +9029,10 @@
         <v>45905</v>
       </c>
       <c r="D16" t="s" s="84">
+        <v>107</v>
+      </c>
+      <c r="E16" t="s" s="84">
         <v>108</v>
-      </c>
-      <c r="E16" t="s" s="84">
-        <v>109</v>
       </c>
       <c r="F16" s="111">
         <v>3640</v>
@@ -9051,10 +9048,10 @@
         <v>1840</v>
       </c>
       <c r="J16" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K16" t="s" s="84">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L16" s="111">
         <v>125</v>
@@ -9084,7 +9081,7 @@
         <v>187</v>
       </c>
       <c r="V16" t="s" s="84">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W16" s="116"/>
       <c r="X16" s="62"/>
@@ -9124,10 +9121,10 @@
         <v>45900</v>
       </c>
       <c r="D17" t="s" s="84">
+        <v>123</v>
+      </c>
+      <c r="E17" t="s" s="84">
         <v>124</v>
-      </c>
-      <c r="E17" t="s" s="84">
-        <v>125</v>
       </c>
       <c r="F17" s="111">
         <v>3615</v>
@@ -9143,10 +9140,10 @@
         <v>1930</v>
       </c>
       <c r="J17" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K17" t="s" s="84">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L17" s="111">
         <v>25</v>
@@ -9176,7 +9173,7 @@
         <v>197</v>
       </c>
       <c r="V17" t="s" s="84">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W17" s="116"/>
       <c r="X17" s="62"/>
@@ -9196,7 +9193,7 @@
         <v>202</v>
       </c>
       <c r="AD17" t="s" s="84">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AE17" s="117"/>
       <c r="AF17" s="48"/>
@@ -9235,10 +9232,10 @@
         <v>4165</v>
       </c>
       <c r="J18" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K18" t="s" s="84">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L18" s="111">
         <v>115</v>
@@ -9268,7 +9265,7 @@
         <v>177</v>
       </c>
       <c r="V18" t="s" s="84">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W18" s="116"/>
       <c r="X18" s="62"/>
@@ -9288,7 +9285,7 @@
         <v>213</v>
       </c>
       <c r="AD18" t="s" s="84">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AE18" s="117"/>
       <c r="AF18" s="48"/>
@@ -9308,10 +9305,10 @@
         <v>45905</v>
       </c>
       <c r="D19" t="s" s="84">
+        <v>107</v>
+      </c>
+      <c r="E19" t="s" s="84">
         <v>108</v>
-      </c>
-      <c r="E19" t="s" s="84">
-        <v>109</v>
       </c>
       <c r="F19" s="111">
         <v>3640</v>
@@ -9327,10 +9324,10 @@
         <v>1840</v>
       </c>
       <c r="J19" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K19" t="s" s="84">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L19" s="111">
         <v>120</v>
@@ -9345,7 +9342,7 @@
       <c r="O19" s="101"/>
       <c r="P19" s="57"/>
       <c r="Q19" t="s" s="84">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="R19" t="s" s="84">
         <v>214</v>
@@ -9354,13 +9351,13 @@
         <v>215</v>
       </c>
       <c r="T19" t="s" s="114">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U19" t="s" s="115">
         <v>187</v>
       </c>
       <c r="V19" t="s" s="84">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="W19" s="116"/>
       <c r="X19" s="62"/>
@@ -9398,10 +9395,10 @@
         <v>45900</v>
       </c>
       <c r="D20" t="s" s="84">
+        <v>123</v>
+      </c>
+      <c r="E20" t="s" s="84">
         <v>124</v>
-      </c>
-      <c r="E20" t="s" s="84">
-        <v>125</v>
       </c>
       <c r="F20" s="111">
         <v>3615</v>
@@ -9417,10 +9414,10 @@
         <v>1930</v>
       </c>
       <c r="J20" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K20" t="s" s="84">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L20" s="111">
         <v>125</v>
@@ -9444,13 +9441,13 @@
         <v>223</v>
       </c>
       <c r="T20" t="s" s="114">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="U20" t="s" s="115">
         <v>197</v>
       </c>
       <c r="V20" t="s" s="84">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W20" s="116"/>
       <c r="X20" s="62"/>
@@ -9491,7 +9488,7 @@
         <v>229</v>
       </c>
       <c r="E21" t="s" s="84">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F21" s="111">
         <v>3510</v>
@@ -9507,10 +9504,10 @@
         <v>2085</v>
       </c>
       <c r="J21" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K21" t="s" s="84">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L21" s="111">
         <v>27</v>
@@ -9525,7 +9522,7 @@
       <c r="O21" s="101"/>
       <c r="P21" s="57"/>
       <c r="Q21" t="s" s="84">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="R21" t="s" s="84">
         <v>230</v>
@@ -9540,7 +9537,7 @@
         <v>233</v>
       </c>
       <c r="V21" t="s" s="84">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="W21" s="116"/>
       <c r="X21" s="62"/>
@@ -9560,7 +9557,7 @@
         <v>238</v>
       </c>
       <c r="AD21" t="s" s="84">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AE21" s="117"/>
       <c r="AF21" s="48"/>
@@ -9599,10 +9596,10 @@
         <v>2085</v>
       </c>
       <c r="J22" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K22" t="s" s="84">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L22" s="111">
         <v>115</v>
@@ -9632,7 +9629,7 @@
         <v>243</v>
       </c>
       <c r="V22" t="s" s="84">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W22" s="116"/>
       <c r="X22" s="62"/>
@@ -9691,10 +9688,10 @@
         <v>2085</v>
       </c>
       <c r="J23" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K23" t="s" s="84">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L23" s="111">
         <v>120</v>
@@ -9724,7 +9721,7 @@
         <v>243</v>
       </c>
       <c r="V23" t="s" s="84">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W23" s="116"/>
       <c r="X23" s="62"/>
@@ -9783,10 +9780,10 @@
         <v>2085</v>
       </c>
       <c r="J24" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K24" t="s" s="84">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L24" s="111">
         <v>125</v>
@@ -9816,7 +9813,7 @@
         <v>265</v>
       </c>
       <c r="V24" t="s" s="84">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W24" s="116"/>
       <c r="X24" s="122"/>
@@ -9836,7 +9833,7 @@
         <v>270</v>
       </c>
       <c r="AD24" t="s" s="84">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AE24" s="117"/>
       <c r="AF24" s="48"/>
@@ -10020,7 +10017,7 @@
     <row r="6" ht="96" customHeight="1">
       <c r="A6" s="71"/>
       <c r="B6" t="s" s="72">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s" s="73">
         <v>273</v>
@@ -10059,13 +10056,13 @@
         <v>283</v>
       </c>
       <c r="B7" t="s" s="84">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s" s="91">
         <v>284</v>
       </c>
       <c r="D7" t="s" s="87">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7" t="s" s="87">
         <v>285</v>
@@ -10095,7 +10092,7 @@
     </row>
     <row r="8" ht="96" customHeight="1">
       <c r="A8" t="s" s="94">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="95" cm="1">
         <f t="array" ref="B8">IF(COUNTA(C8:H8)=0,"",9992+ROW())</f>
@@ -10105,7 +10102,7 @@
         <v>45806</v>
       </c>
       <c r="D8" t="s" s="97">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s" s="97">
         <v>293</v>
@@ -10118,7 +10115,7 @@
       </c>
       <c r="H8" s="107"/>
       <c r="I8" t="s" s="97">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J8" s="98">
         <v>5</v>
@@ -10144,10 +10141,10 @@
         <v>297</v>
       </c>
       <c r="E9" t="s" s="84">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F9" t="s" s="84">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G9" s="110">
         <v>45823</v>
@@ -10156,13 +10153,13 @@
         <v>298</v>
       </c>
       <c r="I9" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J9" s="111">
         <v>505</v>
       </c>
       <c r="K9" t="s" s="84">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L9" t="s" s="84">
         <v>299</v>
@@ -10182,7 +10179,7 @@
         <v>300</v>
       </c>
       <c r="E10" t="s" s="84">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F10" t="s" s="84">
         <v>301</v>
@@ -10194,13 +10191,13 @@
         <v>302</v>
       </c>
       <c r="I10" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J10" s="111">
         <v>140</v>
       </c>
       <c r="K10" t="s" s="84">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L10" t="s" s="84">
         <v>303</v>
@@ -10220,7 +10217,7 @@
         <v>304</v>
       </c>
       <c r="E11" t="s" s="84">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F11" t="s" s="84">
         <v>305</v>
@@ -10232,13 +10229,13 @@
         <v>306</v>
       </c>
       <c r="I11" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J11" s="111">
         <v>75</v>
       </c>
       <c r="K11" t="s" s="84">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L11" t="s" s="84">
         <v>307</v>
@@ -10258,10 +10255,10 @@
         <v>300</v>
       </c>
       <c r="E12" t="s" s="84">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F12" t="s" s="84">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G12" s="110">
         <v>45824</v>
@@ -10270,13 +10267,13 @@
         <v>308</v>
       </c>
       <c r="I12" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J12" s="111">
         <v>515</v>
       </c>
       <c r="K12" t="s" s="84">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L12" t="s" s="84">
         <v>309</v>
@@ -10308,7 +10305,7 @@
         <v>302</v>
       </c>
       <c r="I13" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J13" s="111">
         <v>140</v>
@@ -10346,7 +10343,7 @@
         <v>306</v>
       </c>
       <c r="I14" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J14" s="111">
         <v>75</v>
@@ -10375,7 +10372,7 @@
         <v>180</v>
       </c>
       <c r="F15" t="s" s="84">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G15" s="110">
         <v>45825</v>
@@ -10384,13 +10381,13 @@
         <v>315</v>
       </c>
       <c r="I15" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J15" s="111">
         <v>525</v>
       </c>
       <c r="K15" t="s" s="84">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L15" t="s" s="84">
         <v>316</v>
@@ -10422,7 +10419,7 @@
         <v>302</v>
       </c>
       <c r="I16" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J16" s="111">
         <v>140</v>
@@ -10460,7 +10457,7 @@
         <v>306</v>
       </c>
       <c r="I17" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J17" s="111">
         <v>75</v>
@@ -10489,7 +10486,7 @@
         <v>211</v>
       </c>
       <c r="F18" t="s" s="84">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G18" s="110">
         <v>45826</v>
@@ -10498,7 +10495,7 @@
         <v>320</v>
       </c>
       <c r="I18" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J18" s="111">
         <v>535</v>
@@ -10536,13 +10533,13 @@
         <v>306</v>
       </c>
       <c r="I19" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J19" s="111">
         <v>140</v>
       </c>
       <c r="K19" t="s" s="84">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L19" t="s" s="84">
         <v>322</v>
@@ -10574,7 +10571,7 @@
         <v>320</v>
       </c>
       <c r="I20" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J20" s="111">
         <v>75</v>
@@ -10612,13 +10609,13 @@
         <v>325</v>
       </c>
       <c r="I21" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J21" s="111">
         <v>25</v>
       </c>
       <c r="K21" t="s" s="84">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L21" t="s" s="84">
         <v>326</v>
@@ -10650,7 +10647,7 @@
         <v>302</v>
       </c>
       <c r="I22" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J22" s="111">
         <v>20</v>
@@ -10688,7 +10685,7 @@
         <v>306</v>
       </c>
       <c r="I23" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J23" s="111">
         <v>15</v>
@@ -10726,7 +10723,7 @@
         <v>298</v>
       </c>
       <c r="I24" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J24" s="111">
         <v>10</v>
@@ -10892,16 +10889,16 @@
     <row r="6" ht="96" customHeight="1">
       <c r="A6" s="71"/>
       <c r="B6" t="s" s="72">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s" s="72">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s" s="73">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s" s="73">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s" s="73">
         <v>273</v>
@@ -10945,22 +10942,22 @@
         <v>342</v>
       </c>
       <c r="B7" t="s" s="84">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s" s="84">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s" s="84">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s" s="84">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s" s="91">
         <v>284</v>
       </c>
       <c r="G7" t="s" s="129">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H7" t="s" s="135">
         <v>343</v>
@@ -10984,7 +10981,7 @@
         <v>349</v>
       </c>
       <c r="O7" t="s" s="87">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P7" s="137"/>
       <c r="Q7" s="137"/>
@@ -10995,26 +10992,26 @@
     </row>
     <row r="8" ht="96" customHeight="1">
       <c r="A8" t="s" s="94">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="95" cm="1">
         <f t="array" ref="B8">IF(COUNTA(F8:H8)=0,"",9992+ROW())</f>
         <v>10000</v>
       </c>
       <c r="C8" t="s" s="138">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" t="s" s="97">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" t="s" s="97">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F8" s="96">
         <v>45806</v>
       </c>
       <c r="G8" t="s" s="97">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H8" s="100">
         <v>50</v>
@@ -11058,7 +11055,7 @@
         <v>354</v>
       </c>
       <c r="E9" t="s" s="84">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F9" s="110">
         <v>45806</v>
@@ -11073,22 +11070,22 @@
         <v>355</v>
       </c>
       <c r="J9" t="s" s="84">
+        <v>95</v>
+      </c>
+      <c r="K9" t="s" s="84">
         <v>96</v>
       </c>
-      <c r="K9" t="s" s="84">
+      <c r="L9" t="s" s="84">
         <v>97</v>
       </c>
-      <c r="L9" t="s" s="84">
+      <c r="M9" t="s" s="114">
         <v>98</v>
       </c>
-      <c r="M9" t="s" s="114">
+      <c r="N9" t="s" s="115">
         <v>99</v>
       </c>
-      <c r="N9" t="s" s="115">
-        <v>100</v>
-      </c>
       <c r="O9" t="s" s="84">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P9" s="134"/>
       <c r="Q9" s="134"/>
@@ -11104,13 +11101,13 @@
         <v>10002</v>
       </c>
       <c r="C10" t="s" s="84">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" t="s" s="84">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E10" t="s" s="84">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F10" s="110">
         <v>45807</v>
@@ -11125,22 +11122,22 @@
         <v>356</v>
       </c>
       <c r="J10" t="s" s="84">
+        <v>111</v>
+      </c>
+      <c r="K10" t="s" s="84">
         <v>112</v>
       </c>
-      <c r="K10" t="s" s="84">
+      <c r="L10" t="s" s="84">
         <v>113</v>
       </c>
-      <c r="L10" t="s" s="84">
+      <c r="M10" t="s" s="114">
         <v>114</v>
       </c>
-      <c r="M10" t="s" s="114">
+      <c r="N10" t="s" s="115">
         <v>115</v>
       </c>
-      <c r="N10" t="s" s="115">
-        <v>116</v>
-      </c>
       <c r="O10" t="s" s="84">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P10" s="134"/>
       <c r="Q10" s="134"/>
@@ -11159,10 +11156,10 @@
         <v>357</v>
       </c>
       <c r="D11" t="s" s="84">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E11" t="s" s="84">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F11" s="110">
         <v>45808</v>
@@ -11177,22 +11174,22 @@
         <v>350</v>
       </c>
       <c r="J11" t="s" s="84">
+        <v>126</v>
+      </c>
+      <c r="K11" t="s" s="84">
         <v>127</v>
       </c>
-      <c r="K11" t="s" s="84">
+      <c r="L11" t="s" s="84">
         <v>128</v>
       </c>
-      <c r="L11" t="s" s="84">
+      <c r="M11" t="s" s="114">
         <v>129</v>
       </c>
-      <c r="M11" t="s" s="114">
+      <c r="N11" t="s" s="115">
         <v>130</v>
       </c>
-      <c r="N11" t="s" s="115">
-        <v>131</v>
-      </c>
       <c r="O11" t="s" s="84">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P11" s="134"/>
       <c r="Q11" s="134"/>
@@ -11211,10 +11208,10 @@
         <v>358</v>
       </c>
       <c r="D12" t="s" s="84">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E12" t="s" s="84">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F12" s="110">
         <v>45807</v>
@@ -11229,22 +11226,22 @@
         <v>350</v>
       </c>
       <c r="J12" t="s" s="84">
+        <v>141</v>
+      </c>
+      <c r="K12" t="s" s="84">
         <v>142</v>
       </c>
-      <c r="K12" t="s" s="84">
+      <c r="L12" t="s" s="84">
         <v>143</v>
       </c>
-      <c r="L12" t="s" s="84">
+      <c r="M12" t="s" s="114">
         <v>144</v>
       </c>
-      <c r="M12" t="s" s="114">
-        <v>145</v>
-      </c>
       <c r="N12" t="s" s="115">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O12" t="s" s="84">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P12" s="134"/>
       <c r="Q12" s="134"/>
@@ -11263,10 +11260,10 @@
         <v>359</v>
       </c>
       <c r="D13" t="s" s="84">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E13" t="s" s="84">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F13" s="110">
         <v>45808</v>
@@ -11290,7 +11287,7 @@
         <v>155</v>
       </c>
       <c r="M13" t="s" s="114">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N13" t="s" s="115">
         <v>156</v>
@@ -11315,10 +11312,10 @@
         <v>360</v>
       </c>
       <c r="D14" t="s" s="84">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E14" t="s" s="84">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F14" s="110">
         <v>45809</v>
@@ -11342,7 +11339,7 @@
         <v>165</v>
       </c>
       <c r="M14" t="s" s="114">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N14" t="s" s="115">
         <v>166</v>
@@ -11367,7 +11364,7 @@
         <v>361</v>
       </c>
       <c r="D15" t="s" s="84">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E15" t="s" s="84">
         <v>173</v>
@@ -11385,7 +11382,7 @@
         <v>350</v>
       </c>
       <c r="J15" t="s" s="84">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K15" t="s" s="84">
         <v>175</v>
@@ -11394,7 +11391,7 @@
         <v>176</v>
       </c>
       <c r="M15" t="s" s="114">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N15" t="s" s="115">
         <v>177</v>
@@ -11422,7 +11419,7 @@
         <v>174</v>
       </c>
       <c r="E16" t="s" s="84">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F16" s="110">
         <v>45809</v>
@@ -11471,10 +11468,10 @@
         <v>363</v>
       </c>
       <c r="D17" t="s" s="84">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E17" t="s" s="84">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F17" s="110">
         <v>45810</v>
@@ -11504,7 +11501,7 @@
         <v>197</v>
       </c>
       <c r="O17" t="s" s="84">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P17" s="134"/>
       <c r="Q17" s="134"/>
@@ -11523,7 +11520,7 @@
         <v>364</v>
       </c>
       <c r="D18" t="s" s="84">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E18" t="s" s="84">
         <v>203</v>
@@ -11556,7 +11553,7 @@
         <v>177</v>
       </c>
       <c r="O18" t="s" s="84">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P18" s="134"/>
       <c r="Q18" s="134"/>
@@ -11578,7 +11575,7 @@
         <v>204</v>
       </c>
       <c r="E19" t="s" s="84">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F19" s="110">
         <v>45810</v>
@@ -11593,7 +11590,7 @@
         <v>350</v>
       </c>
       <c r="J19" t="s" s="84">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K19" t="s" s="84">
         <v>214</v>
@@ -11602,7 +11599,7 @@
         <v>215</v>
       </c>
       <c r="M19" t="s" s="114">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N19" t="s" s="115">
         <v>187</v>
@@ -11625,10 +11622,10 @@
         <v>366</v>
       </c>
       <c r="D20" t="s" s="84">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E20" t="s" s="84">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F20" s="110">
         <v>45811</v>
@@ -11652,7 +11649,7 @@
         <v>223</v>
       </c>
       <c r="M20" t="s" s="114">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N20" t="s" s="115">
         <v>197</v>
@@ -11675,7 +11672,7 @@
         <v>367</v>
       </c>
       <c r="D21" t="s" s="84">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E21" t="s" s="84">
         <v>229</v>
@@ -11693,7 +11690,7 @@
         <v>356</v>
       </c>
       <c r="J21" t="s" s="84">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K21" t="s" s="84">
         <v>230</v>
@@ -11708,7 +11705,7 @@
         <v>233</v>
       </c>
       <c r="O21" t="s" s="84">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P21" s="134"/>
       <c r="Q21" s="134"/>
@@ -11727,7 +11724,7 @@
         <v>368</v>
       </c>
       <c r="D22" t="s" s="84">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E22" t="s" s="84">
         <v>173</v>
@@ -11864,7 +11861,7 @@
         <v>265</v>
       </c>
       <c r="O24" t="s" s="84">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P24" s="140"/>
       <c r="Q24" s="140"/>
@@ -11938,7 +11935,7 @@
   <sheetData>
     <row r="1" s="143" customFormat="1" ht="29" customHeight="1">
       <c r="A1" t="s" s="144">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s" s="144">
         <v>371</v>
@@ -12130,7 +12127,7 @@
         <v>433</v>
       </c>
       <c r="BM1" t="s" s="144">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BN1" t="s" s="144">
         <v>434</v>
@@ -12166,7 +12163,7 @@
         <v>249</v>
       </c>
       <c r="BY1" t="s" s="144">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BZ1" t="s" s="144">
         <v>444</v>
@@ -14568,7 +14565,7 @@
     </row>
     <row r="2" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A2" t="s" s="144">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s" s="144">
         <v>1196</v>
@@ -14619,10 +14616,10 @@
         <v>1211</v>
       </c>
       <c r="R2" t="s" s="144">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S2" t="s" s="144">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T2" t="s" s="144">
         <v>1212</v>
@@ -14637,7 +14634,7 @@
         <v>1214</v>
       </c>
       <c r="X2" t="s" s="144">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Y2" t="s" s="144">
         <v>1215</v>
@@ -14655,7 +14652,7 @@
         <v>204</v>
       </c>
       <c r="AD2" t="s" s="144">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AE2" t="s" s="144">
         <v>174</v>
@@ -14744,7 +14741,7 @@
     </row>
     <row r="15" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A15" t="s" s="144">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s" s="144">
         <v>1237</v>
@@ -14752,7 +14749,7 @@
     </row>
     <row r="16" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A16" t="s" s="144">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s" s="144">
         <v>1238</v>
@@ -14760,7 +14757,7 @@
     </row>
     <row r="17" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A17" t="s" s="144">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s" s="144">
         <v>1239</v>
@@ -14768,7 +14765,7 @@
     </row>
     <row r="18" s="143" customFormat="1" ht="42" customHeight="1">
       <c r="A18" t="s" s="156">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s" s="144">
         <v>1240</v>
@@ -14776,7 +14773,7 @@
     </row>
     <row r="19" s="143" customFormat="1" ht="29" customHeight="1">
       <c r="A19" t="s" s="156">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s" s="144">
         <v>1241</v>
@@ -14784,7 +14781,7 @@
     </row>
     <row r="20" s="143" customFormat="1" ht="29" customHeight="1">
       <c r="A20" t="s" s="156">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s" s="144">
         <v>1242</v>
@@ -14792,7 +14789,7 @@
     </row>
     <row r="21" s="143" customFormat="1" ht="42" customHeight="1">
       <c r="A21" t="s" s="156">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s" s="144">
         <v>1243</v>
@@ -14800,7 +14797,7 @@
     </row>
     <row r="22" s="143" customFormat="1" ht="29" customHeight="1">
       <c r="A22" t="s" s="156">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s" s="144">
         <v>1244</v>
@@ -14808,7 +14805,7 @@
     </row>
     <row r="23" s="143" customFormat="1" ht="55" customHeight="1">
       <c r="A23" t="s" s="156">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s" s="144">
         <v>1245</v>
@@ -14816,7 +14813,7 @@
     </row>
     <row r="24" s="143" customFormat="1" ht="42" customHeight="1">
       <c r="A24" t="s" s="156">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s" s="144">
         <v>1246</v>
@@ -14824,7 +14821,7 @@
     </row>
     <row r="25" s="143" customFormat="1" ht="42" customHeight="1">
       <c r="A25" t="s" s="156">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s" s="144">
         <v>1247</v>
@@ -14832,7 +14829,7 @@
     </row>
     <row r="26" s="143" customFormat="1" ht="29" customHeight="1">
       <c r="A26" t="s" s="156">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s" s="144">
         <v>1248</v>
@@ -14840,7 +14837,7 @@
     </row>
     <row r="27" s="143" customFormat="1" ht="42" customHeight="1">
       <c r="A27" t="s" s="156">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s" s="144">
         <v>1249</v>
@@ -14848,7 +14845,7 @@
     </row>
     <row r="30" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A30" t="s" s="144">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s" s="144">
         <v>1250</v>
@@ -14856,7 +14853,7 @@
     </row>
     <row r="31" s="143" customFormat="1" ht="29" customHeight="1">
       <c r="A31" t="s" s="156">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s" s="144">
         <v>1251</v>
@@ -14864,7 +14861,7 @@
     </row>
     <row r="32" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A32" t="s" s="144">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s" s="144">
         <v>1252</v>
@@ -14872,7 +14869,7 @@
     </row>
     <row r="33" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A33" t="s" s="144">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s" s="144">
         <v>1253</v>
@@ -14880,7 +14877,7 @@
     </row>
     <row r="34" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A34" t="s" s="144">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" t="s" s="144">
         <v>1254</v>
@@ -14888,7 +14885,7 @@
     </row>
     <row r="35" s="143" customFormat="1" ht="55" customHeight="1">
       <c r="A35" t="s" s="156">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s" s="144">
         <v>1255</v>
@@ -14902,7 +14899,7 @@
     </row>
     <row r="39" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A39" t="s" s="144">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B39" t="s" s="144">
         <v>1237</v>
@@ -14990,7 +14987,7 @@
     </row>
     <row r="52" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A52" t="s" s="144">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B52" t="s" s="144">
         <v>1237</v>
@@ -14998,7 +14995,7 @@
     </row>
     <row r="53" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A53" t="s" s="144">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B53" t="s" s="144">
         <v>1266</v>
@@ -15006,7 +15003,7 @@
     </row>
     <row r="54" s="143" customFormat="1" ht="42" customHeight="1">
       <c r="A54" t="s" s="156">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B54" t="s" s="144">
         <v>1240</v>
@@ -15014,7 +15011,7 @@
     </row>
     <row r="55" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A55" t="s" s="144">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B55" t="s" s="144">
         <v>1239</v>
@@ -15097,7 +15094,7 @@
         <v>341</v>
       </c>
       <c r="B65" t="s" s="144">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PAE-448: Introduces Summary Log validation check for missing rows (#341)
</commit_message>
<xml_diff>
--- a/src/data/fixtures/uploads/reprocessor.xlsx
+++ b/src/data/fixtures/uploads/reprocessor.xlsx
@@ -188,9 +188,6 @@
     <t>__EPR_META_ACCREDITATION</t>
   </si>
   <si>
-    <t>68f6a147c117aec8a1ab7495</t>
-  </si>
-  <si>
     <t>__EPR_META_REGISTRATION</t>
   </si>
   <si>
@@ -681,6 +678,9 @@
   </si>
   <si>
     <t>Actual weight (100%)</t>
+  </si>
+  <si>
+    <t>Calc</t>
   </si>
   <si>
     <t>A W Jenkinson Woodwaste Ltd</t>
@@ -6818,14 +6818,12 @@
       <c r="C12" t="s" s="22">
         <v>11</v>
       </c>
-      <c r="D12" t="s" s="21">
+      <c r="D12" s="21"/>
+      <c r="E12" t="s" s="22">
         <v>12</v>
       </c>
-      <c r="E12" t="s" s="22">
+      <c r="F12" t="s" s="21">
         <v>13</v>
-      </c>
-      <c r="F12" t="s" s="21">
-        <v>14</v>
       </c>
       <c r="G12" s="23"/>
       <c r="H12" s="9"/>
@@ -7937,7 +7935,7 @@
       <c r="AB2" s="36"/>
       <c r="AC2" s="36"/>
       <c r="AD2" t="s" s="37">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AE2" s="38"/>
       <c r="AF2" s="38"/>
@@ -7950,7 +7948,7 @@
     <row r="3" ht="56.1" customHeight="1">
       <c r="A3" s="6"/>
       <c r="B3" t="s" s="40">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="41"/>
       <c r="D3" s="42"/>
@@ -7967,26 +7965,26 @@
       <c r="O3" s="9"/>
       <c r="P3" s="35"/>
       <c r="Q3" t="s" s="43">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R3" s="44"/>
       <c r="S3" s="45"/>
       <c r="T3" s="35"/>
       <c r="U3" t="s" s="46">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V3" s="35"/>
       <c r="W3" s="31"/>
       <c r="X3" s="36"/>
       <c r="Y3" t="s" s="43">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Z3" s="44"/>
       <c r="AA3" s="47"/>
       <c r="AB3" s="47"/>
       <c r="AC3" s="47"/>
       <c r="AD3" t="s" s="37">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AE3" s="48"/>
       <c r="AF3" s="48"/>
@@ -7999,13 +7997,13 @@
     <row r="4" ht="56.1" customHeight="1">
       <c r="A4" s="50"/>
       <c r="B4" t="s" s="51">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="53"/>
       <c r="E4" s="54"/>
       <c r="F4" t="s" s="55">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="56"/>
       <c r="H4" s="56"/>
@@ -8018,19 +8016,19 @@
       <c r="O4" s="9"/>
       <c r="P4" s="57"/>
       <c r="Q4" t="s" s="58">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R4" s="59"/>
       <c r="S4" s="60"/>
       <c r="T4" s="61"/>
       <c r="U4" t="s" s="46">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V4" s="35"/>
       <c r="W4" s="31"/>
       <c r="X4" s="62"/>
       <c r="Y4" t="s" s="63">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Z4" s="64"/>
       <c r="AA4" s="64"/>
@@ -8087,43 +8085,43 @@
     <row r="6" ht="96" customHeight="1">
       <c r="A6" s="71"/>
       <c r="B6" t="s" s="72">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s" s="73">
         <v>26</v>
       </c>
-      <c r="C6" t="s" s="73">
+      <c r="D6" t="s" s="73">
         <v>27</v>
       </c>
-      <c r="D6" t="s" s="73">
+      <c r="E6" t="s" s="73">
         <v>28</v>
       </c>
-      <c r="E6" t="s" s="73">
+      <c r="F6" t="s" s="73">
         <v>29</v>
       </c>
-      <c r="F6" t="s" s="73">
+      <c r="G6" t="s" s="73">
         <v>30</v>
       </c>
-      <c r="G6" t="s" s="73">
+      <c r="H6" t="s" s="73">
         <v>31</v>
       </c>
-      <c r="H6" t="s" s="73">
+      <c r="I6" t="s" s="73">
         <v>32</v>
       </c>
-      <c r="I6" t="s" s="73">
+      <c r="J6" t="s" s="73">
         <v>33</v>
       </c>
-      <c r="J6" t="s" s="73">
+      <c r="K6" t="s" s="73">
         <v>34</v>
       </c>
-      <c r="K6" t="s" s="73">
+      <c r="L6" t="s" s="73">
         <v>35</v>
       </c>
-      <c r="L6" t="s" s="73">
+      <c r="M6" t="s" s="73">
         <v>36</v>
       </c>
-      <c r="M6" t="s" s="73">
+      <c r="N6" t="s" s="73">
         <v>37</v>
-      </c>
-      <c r="N6" t="s" s="73">
-        <v>38</v>
       </c>
       <c r="O6" s="74">
         <v>1</v>
@@ -8132,22 +8130,22 @@
         <v>2</v>
       </c>
       <c r="Q6" t="s" s="76">
+        <v>38</v>
+      </c>
+      <c r="R6" t="s" s="76">
         <v>39</v>
       </c>
-      <c r="R6" t="s" s="76">
+      <c r="S6" t="s" s="76">
         <v>40</v>
       </c>
-      <c r="S6" t="s" s="76">
+      <c r="T6" t="s" s="76">
         <v>41</v>
       </c>
-      <c r="T6" t="s" s="76">
+      <c r="U6" t="s" s="77">
         <v>42</v>
       </c>
-      <c r="U6" t="s" s="77">
+      <c r="V6" t="s" s="76">
         <v>43</v>
-      </c>
-      <c r="V6" t="s" s="76">
-        <v>44</v>
       </c>
       <c r="W6" s="78">
         <v>3</v>
@@ -8156,22 +8154,22 @@
         <v>4</v>
       </c>
       <c r="Y6" t="s" s="73">
+        <v>44</v>
+      </c>
+      <c r="Z6" t="s" s="76">
         <v>45</v>
       </c>
-      <c r="Z6" t="s" s="76">
+      <c r="AA6" t="s" s="76">
         <v>46</v>
       </c>
-      <c r="AA6" t="s" s="76">
+      <c r="AB6" t="s" s="76">
         <v>47</v>
       </c>
-      <c r="AB6" t="s" s="76">
+      <c r="AC6" t="s" s="76">
         <v>48</v>
       </c>
-      <c r="AC6" t="s" s="76">
+      <c r="AD6" t="s" s="76">
         <v>49</v>
-      </c>
-      <c r="AD6" t="s" s="76">
-        <v>50</v>
       </c>
       <c r="AE6" s="80">
         <v>5</v>
@@ -8185,94 +8183,94 @@
     </row>
     <row r="7" ht="48.75" customHeight="1">
       <c r="A7" t="s" s="83">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s" s="84">
         <v>51</v>
       </c>
-      <c r="B7" t="s" s="84">
+      <c r="C7" t="s" s="84">
         <v>52</v>
       </c>
-      <c r="C7" t="s" s="84">
+      <c r="D7" t="s" s="84">
         <v>53</v>
       </c>
-      <c r="D7" t="s" s="84">
+      <c r="E7" t="s" s="84">
         <v>54</v>
       </c>
-      <c r="E7" t="s" s="84">
+      <c r="F7" t="s" s="84">
         <v>55</v>
       </c>
-      <c r="F7" t="s" s="84">
+      <c r="G7" t="s" s="84">
         <v>56</v>
       </c>
-      <c r="G7" t="s" s="84">
+      <c r="H7" t="s" s="84">
         <v>57</v>
       </c>
-      <c r="H7" t="s" s="84">
+      <c r="I7" t="s" s="84">
         <v>58</v>
       </c>
-      <c r="I7" t="s" s="84">
+      <c r="J7" t="s" s="84">
         <v>59</v>
       </c>
-      <c r="J7" t="s" s="84">
+      <c r="K7" t="s" s="84">
         <v>60</v>
       </c>
-      <c r="K7" t="s" s="84">
+      <c r="L7" t="s" s="84">
         <v>61</v>
       </c>
-      <c r="L7" t="s" s="84">
+      <c r="M7" t="s" s="84">
         <v>62</v>
       </c>
-      <c r="M7" t="s" s="84">
+      <c r="N7" t="s" s="84">
         <v>63</v>
       </c>
-      <c r="N7" t="s" s="84">
+      <c r="O7" t="s" s="85">
         <v>64</v>
       </c>
-      <c r="O7" t="s" s="85">
+      <c r="P7" t="s" s="86">
         <v>65</v>
       </c>
-      <c r="P7" t="s" s="86">
+      <c r="Q7" t="s" s="87">
         <v>66</v>
       </c>
-      <c r="Q7" t="s" s="87">
+      <c r="R7" t="s" s="87">
         <v>67</v>
       </c>
-      <c r="R7" t="s" s="87">
+      <c r="S7" t="s" s="87">
         <v>68</v>
       </c>
-      <c r="S7" t="s" s="87">
+      <c r="T7" t="s" s="87">
         <v>69</v>
       </c>
-      <c r="T7" t="s" s="87">
+      <c r="U7" t="s" s="88">
         <v>70</v>
       </c>
-      <c r="U7" t="s" s="88">
+      <c r="V7" t="s" s="87">
         <v>71</v>
       </c>
-      <c r="V7" t="s" s="87">
+      <c r="W7" t="s" s="89">
+        <v>64</v>
+      </c>
+      <c r="X7" t="s" s="90">
         <v>72</v>
       </c>
-      <c r="W7" t="s" s="89">
-        <v>65</v>
-      </c>
-      <c r="X7" t="s" s="90">
+      <c r="Y7" t="s" s="91">
         <v>73</v>
       </c>
-      <c r="Y7" t="s" s="91">
+      <c r="Z7" t="s" s="87">
         <v>74</v>
       </c>
-      <c r="Z7" t="s" s="87">
+      <c r="AA7" t="s" s="87">
         <v>75</v>
       </c>
-      <c r="AA7" t="s" s="87">
+      <c r="AB7" t="s" s="87">
         <v>76</v>
       </c>
-      <c r="AB7" t="s" s="87">
+      <c r="AC7" t="s" s="87">
         <v>77</v>
       </c>
-      <c r="AC7" t="s" s="87">
+      <c r="AD7" t="s" s="87">
         <v>78</v>
-      </c>
-      <c r="AD7" t="s" s="87">
-        <v>79</v>
       </c>
       <c r="AE7" s="92"/>
       <c r="AF7" s="92"/>
@@ -8284,7 +8282,7 @@
     </row>
     <row r="8" ht="96" customHeight="1">
       <c r="A8" t="s" s="94">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="95" cm="1">
         <f t="array" ref="B8">IF(COUNTA(F8:G8)=0,"",9992+ROW())</f>
@@ -8294,10 +8292,10 @@
         <v>45805</v>
       </c>
       <c r="D8" t="s" s="97">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" t="s" s="97">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F8" s="98">
         <v>50</v>
@@ -8313,10 +8311,10 @@
         <v>30</v>
       </c>
       <c r="J8" t="s" s="97">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K8" t="s" s="97">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L8" s="98">
         <v>5</v>
@@ -8330,44 +8328,44 @@
       </c>
       <c r="O8" s="101"/>
       <c r="P8" t="s" s="102">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q8" t="s" s="97">
+        <v>82</v>
+      </c>
+      <c r="R8" t="s" s="97">
         <v>83</v>
       </c>
-      <c r="R8" t="s" s="97">
+      <c r="S8" t="s" s="97">
         <v>84</v>
       </c>
-      <c r="S8" t="s" s="97">
+      <c r="T8" t="s" s="103">
         <v>85</v>
-      </c>
-      <c r="T8" t="s" s="103">
-        <v>86</v>
       </c>
       <c r="U8" s="104">
         <v>1234567890</v>
       </c>
       <c r="V8" t="s" s="97">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="W8" s="105"/>
       <c r="X8" t="s" s="106">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Y8" t="s" s="97">
+        <v>87</v>
+      </c>
+      <c r="Z8" t="s" s="97">
         <v>88</v>
       </c>
-      <c r="Z8" t="s" s="97">
+      <c r="AA8" t="s" s="97">
         <v>89</v>
       </c>
-      <c r="AA8" t="s" s="97">
+      <c r="AB8" t="s" s="97">
         <v>90</v>
       </c>
-      <c r="AB8" t="s" s="97">
+      <c r="AC8" t="s" s="97">
         <v>91</v>
-      </c>
-      <c r="AC8" t="s" s="97">
-        <v>92</v>
       </c>
       <c r="AD8" s="107"/>
       <c r="AE8" s="108"/>
@@ -8388,10 +8386,10 @@
         <v>45870</v>
       </c>
       <c r="D9" t="s" s="84">
+        <v>92</v>
+      </c>
+      <c r="E9" t="s" s="84">
         <v>93</v>
-      </c>
-      <c r="E9" t="s" s="84">
-        <v>94</v>
       </c>
       <c r="F9" s="111">
         <v>10000</v>
@@ -8407,10 +8405,10 @@
         <v>4495</v>
       </c>
       <c r="J9" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K9" t="s" s="84">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L9" s="111">
         <v>21</v>
@@ -8425,42 +8423,42 @@
       <c r="O9" s="101"/>
       <c r="P9" s="57"/>
       <c r="Q9" t="s" s="84">
+        <v>95</v>
+      </c>
+      <c r="R9" t="s" s="84">
         <v>96</v>
       </c>
-      <c r="R9" t="s" s="84">
+      <c r="S9" t="s" s="84">
         <v>97</v>
       </c>
-      <c r="S9" t="s" s="84">
+      <c r="T9" t="s" s="114">
         <v>98</v>
       </c>
-      <c r="T9" t="s" s="114">
+      <c r="U9" t="s" s="115">
         <v>99</v>
       </c>
-      <c r="U9" t="s" s="115">
+      <c r="V9" t="s" s="84">
         <v>100</v>
-      </c>
-      <c r="V9" t="s" s="84">
-        <v>101</v>
       </c>
       <c r="W9" s="116"/>
       <c r="X9" s="62"/>
       <c r="Y9" t="s" s="84">
+        <v>101</v>
+      </c>
+      <c r="Z9" t="s" s="84">
         <v>102</v>
       </c>
-      <c r="Z9" t="s" s="84">
+      <c r="AA9" t="s" s="84">
         <v>103</v>
       </c>
-      <c r="AA9" t="s" s="84">
+      <c r="AB9" t="s" s="84">
         <v>104</v>
       </c>
-      <c r="AB9" t="s" s="84">
+      <c r="AC9" t="s" s="84">
         <v>105</v>
       </c>
-      <c r="AC9" t="s" s="84">
+      <c r="AD9" t="s" s="84">
         <v>106</v>
-      </c>
-      <c r="AD9" t="s" s="84">
-        <v>107</v>
       </c>
       <c r="AE9" s="117"/>
       <c r="AF9" s="48"/>
@@ -8480,10 +8478,10 @@
         <v>45905</v>
       </c>
       <c r="D10" t="s" s="84">
+        <v>107</v>
+      </c>
+      <c r="E10" t="s" s="84">
         <v>108</v>
-      </c>
-      <c r="E10" t="s" s="84">
-        <v>109</v>
       </c>
       <c r="F10" s="111">
         <v>3640</v>
@@ -8499,10 +8497,10 @@
         <v>1840</v>
       </c>
       <c r="J10" t="s" s="84">
+        <v>109</v>
+      </c>
+      <c r="K10" t="s" s="84">
         <v>110</v>
-      </c>
-      <c r="K10" t="s" s="84">
-        <v>111</v>
       </c>
       <c r="L10" s="111">
         <v>115</v>
@@ -8517,42 +8515,42 @@
       <c r="O10" s="101"/>
       <c r="P10" s="57"/>
       <c r="Q10" t="s" s="84">
+        <v>111</v>
+      </c>
+      <c r="R10" t="s" s="84">
         <v>112</v>
       </c>
-      <c r="R10" t="s" s="84">
+      <c r="S10" t="s" s="84">
         <v>113</v>
       </c>
-      <c r="S10" t="s" s="84">
+      <c r="T10" t="s" s="114">
         <v>114</v>
       </c>
-      <c r="T10" t="s" s="114">
+      <c r="U10" t="s" s="115">
         <v>115</v>
       </c>
-      <c r="U10" t="s" s="115">
+      <c r="V10" t="s" s="84">
         <v>116</v>
-      </c>
-      <c r="V10" t="s" s="84">
-        <v>117</v>
       </c>
       <c r="W10" s="116"/>
       <c r="X10" s="62"/>
       <c r="Y10" t="s" s="84">
+        <v>117</v>
+      </c>
+      <c r="Z10" t="s" s="84">
         <v>118</v>
       </c>
-      <c r="Z10" t="s" s="84">
+      <c r="AA10" t="s" s="84">
         <v>119</v>
       </c>
-      <c r="AA10" t="s" s="84">
+      <c r="AB10" t="s" s="84">
         <v>120</v>
       </c>
-      <c r="AB10" t="s" s="84">
+      <c r="AC10" t="s" s="84">
         <v>121</v>
       </c>
-      <c r="AC10" t="s" s="84">
+      <c r="AD10" t="s" s="84">
         <v>122</v>
-      </c>
-      <c r="AD10" t="s" s="84">
-        <v>123</v>
       </c>
       <c r="AE10" s="117"/>
       <c r="AF10" s="48"/>
@@ -8572,10 +8570,10 @@
         <v>45900</v>
       </c>
       <c r="D11" t="s" s="84">
+        <v>123</v>
+      </c>
+      <c r="E11" t="s" s="84">
         <v>124</v>
-      </c>
-      <c r="E11" t="s" s="84">
-        <v>125</v>
       </c>
       <c r="F11" s="111">
         <v>3615</v>
@@ -8591,10 +8589,10 @@
         <v>1930</v>
       </c>
       <c r="J11" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K11" t="s" s="84">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L11" s="111">
         <v>120</v>
@@ -8609,42 +8607,42 @@
       <c r="O11" s="101"/>
       <c r="P11" s="57"/>
       <c r="Q11" t="s" s="84">
+        <v>126</v>
+      </c>
+      <c r="R11" t="s" s="84">
         <v>127</v>
       </c>
-      <c r="R11" t="s" s="84">
+      <c r="S11" t="s" s="84">
         <v>128</v>
       </c>
-      <c r="S11" t="s" s="84">
+      <c r="T11" t="s" s="114">
         <v>129</v>
       </c>
-      <c r="T11" t="s" s="114">
+      <c r="U11" t="s" s="115">
         <v>130</v>
       </c>
-      <c r="U11" t="s" s="115">
+      <c r="V11" t="s" s="84">
         <v>131</v>
-      </c>
-      <c r="V11" t="s" s="84">
-        <v>132</v>
       </c>
       <c r="W11" s="116"/>
       <c r="X11" s="62"/>
       <c r="Y11" t="s" s="84">
+        <v>132</v>
+      </c>
+      <c r="Z11" t="s" s="84">
         <v>133</v>
       </c>
-      <c r="Z11" t="s" s="84">
+      <c r="AA11" t="s" s="84">
         <v>134</v>
       </c>
-      <c r="AA11" t="s" s="84">
+      <c r="AB11" t="s" s="84">
         <v>135</v>
       </c>
-      <c r="AB11" t="s" s="84">
+      <c r="AC11" t="s" s="84">
         <v>136</v>
       </c>
-      <c r="AC11" t="s" s="84">
+      <c r="AD11" t="s" s="84">
         <v>137</v>
-      </c>
-      <c r="AD11" t="s" s="84">
-        <v>138</v>
       </c>
       <c r="AE11" s="117"/>
       <c r="AF11" s="48"/>
@@ -8664,10 +8662,10 @@
         <v>45871</v>
       </c>
       <c r="D12" t="s" s="84">
+        <v>138</v>
+      </c>
+      <c r="E12" t="s" s="84">
         <v>139</v>
-      </c>
-      <c r="E12" t="s" s="84">
-        <v>140</v>
       </c>
       <c r="F12" s="111">
         <v>10050</v>
@@ -8683,10 +8681,10 @@
         <v>4385</v>
       </c>
       <c r="J12" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K12" t="s" s="84">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L12" s="111">
         <v>125</v>
@@ -8701,42 +8699,42 @@
       <c r="O12" s="101"/>
       <c r="P12" s="57"/>
       <c r="Q12" t="s" s="84">
+        <v>141</v>
+      </c>
+      <c r="R12" t="s" s="84">
         <v>142</v>
       </c>
-      <c r="R12" t="s" s="84">
+      <c r="S12" t="s" s="84">
         <v>143</v>
       </c>
-      <c r="S12" t="s" s="84">
+      <c r="T12" t="s" s="114">
         <v>144</v>
       </c>
-      <c r="T12" t="s" s="114">
+      <c r="U12" t="s" s="115">
+        <v>99</v>
+      </c>
+      <c r="V12" t="s" s="84">
         <v>145</v>
-      </c>
-      <c r="U12" t="s" s="115">
-        <v>100</v>
-      </c>
-      <c r="V12" t="s" s="84">
-        <v>146</v>
       </c>
       <c r="W12" s="116"/>
       <c r="X12" s="62"/>
       <c r="Y12" t="s" s="84">
+        <v>146</v>
+      </c>
+      <c r="Z12" t="s" s="84">
         <v>147</v>
       </c>
-      <c r="Z12" t="s" s="84">
+      <c r="AA12" t="s" s="84">
         <v>148</v>
       </c>
-      <c r="AA12" t="s" s="84">
+      <c r="AB12" t="s" s="84">
         <v>149</v>
       </c>
-      <c r="AB12" t="s" s="84">
+      <c r="AC12" t="s" s="84">
         <v>150</v>
       </c>
-      <c r="AC12" t="s" s="84">
-        <v>151</v>
-      </c>
       <c r="AD12" t="s" s="84">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AE12" s="117"/>
       <c r="AF12" s="48"/>
@@ -8756,10 +8754,10 @@
         <v>45905</v>
       </c>
       <c r="D13" t="s" s="84">
+        <v>107</v>
+      </c>
+      <c r="E13" t="s" s="84">
         <v>108</v>
-      </c>
-      <c r="E13" t="s" s="84">
-        <v>109</v>
       </c>
       <c r="F13" s="111">
         <v>3640</v>
@@ -8775,10 +8773,10 @@
         <v>1840</v>
       </c>
       <c r="J13" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K13" t="s" s="84">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L13" s="111">
         <v>23</v>
@@ -8786,9 +8784,8 @@
       <c r="M13" s="113">
         <v>0.95</v>
       </c>
-      <c r="N13" s="111" cm="1">
-        <f t="array" ref="N13">_xlfn.IFERROR((IF(IF(J13="Yes",((I13-(I13*0.15%))*M13),(I13*M13))=0,"",IF(J13="Yes",((I13-(I13*0.15%))*M13),(I13*M13)))-L13),"")</f>
-        <v>1722.378</v>
+      <c r="N13" t="s" s="84">
+        <v>152</v>
       </c>
       <c r="O13" s="101"/>
       <c r="P13" s="57"/>
@@ -8802,13 +8799,13 @@
         <v>155</v>
       </c>
       <c r="T13" t="s" s="114">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="U13" t="s" s="115">
         <v>156</v>
       </c>
       <c r="V13" t="s" s="84">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W13" s="116"/>
       <c r="X13" s="62"/>
@@ -8848,10 +8845,10 @@
         <v>45900</v>
       </c>
       <c r="D14" t="s" s="84">
+        <v>123</v>
+      </c>
+      <c r="E14" t="s" s="84">
         <v>124</v>
-      </c>
-      <c r="E14" t="s" s="84">
-        <v>125</v>
       </c>
       <c r="F14" s="111">
         <v>3615</v>
@@ -8867,10 +8864,10 @@
         <v>1930</v>
       </c>
       <c r="J14" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K14" t="s" s="84">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L14" s="111">
         <v>115</v>
@@ -8894,13 +8891,13 @@
         <v>165</v>
       </c>
       <c r="T14" t="s" s="114">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="U14" t="s" s="115">
         <v>166</v>
       </c>
       <c r="V14" t="s" s="84">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="W14" s="116"/>
       <c r="X14" s="62"/>
@@ -8959,10 +8956,10 @@
         <v>4275</v>
       </c>
       <c r="J15" t="s" s="84">
+        <v>109</v>
+      </c>
+      <c r="K15" t="s" s="84">
         <v>110</v>
-      </c>
-      <c r="K15" t="s" s="84">
-        <v>111</v>
       </c>
       <c r="L15" s="111">
         <v>120</v>
@@ -8977,7 +8974,7 @@
       <c r="O15" s="101"/>
       <c r="P15" s="57"/>
       <c r="Q15" t="s" s="84">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="R15" t="s" s="84">
         <v>175</v>
@@ -8986,13 +8983,13 @@
         <v>176</v>
       </c>
       <c r="T15" t="s" s="114">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="U15" t="s" s="115">
         <v>177</v>
       </c>
       <c r="V15" t="s" s="84">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W15" s="116"/>
       <c r="X15" s="62"/>
@@ -9032,10 +9029,10 @@
         <v>45905</v>
       </c>
       <c r="D16" t="s" s="84">
+        <v>107</v>
+      </c>
+      <c r="E16" t="s" s="84">
         <v>108</v>
-      </c>
-      <c r="E16" t="s" s="84">
-        <v>109</v>
       </c>
       <c r="F16" s="111">
         <v>3640</v>
@@ -9051,10 +9048,10 @@
         <v>1840</v>
       </c>
       <c r="J16" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K16" t="s" s="84">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L16" s="111">
         <v>125</v>
@@ -9084,7 +9081,7 @@
         <v>187</v>
       </c>
       <c r="V16" t="s" s="84">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W16" s="116"/>
       <c r="X16" s="62"/>
@@ -9124,10 +9121,10 @@
         <v>45900</v>
       </c>
       <c r="D17" t="s" s="84">
+        <v>123</v>
+      </c>
+      <c r="E17" t="s" s="84">
         <v>124</v>
-      </c>
-      <c r="E17" t="s" s="84">
-        <v>125</v>
       </c>
       <c r="F17" s="111">
         <v>3615</v>
@@ -9143,10 +9140,10 @@
         <v>1930</v>
       </c>
       <c r="J17" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K17" t="s" s="84">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L17" s="111">
         <v>25</v>
@@ -9176,7 +9173,7 @@
         <v>197</v>
       </c>
       <c r="V17" t="s" s="84">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W17" s="116"/>
       <c r="X17" s="62"/>
@@ -9196,7 +9193,7 @@
         <v>202</v>
       </c>
       <c r="AD17" t="s" s="84">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AE17" s="117"/>
       <c r="AF17" s="48"/>
@@ -9235,10 +9232,10 @@
         <v>4165</v>
       </c>
       <c r="J18" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K18" t="s" s="84">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L18" s="111">
         <v>115</v>
@@ -9268,7 +9265,7 @@
         <v>177</v>
       </c>
       <c r="V18" t="s" s="84">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W18" s="116"/>
       <c r="X18" s="62"/>
@@ -9288,7 +9285,7 @@
         <v>213</v>
       </c>
       <c r="AD18" t="s" s="84">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AE18" s="117"/>
       <c r="AF18" s="48"/>
@@ -9308,10 +9305,10 @@
         <v>45905</v>
       </c>
       <c r="D19" t="s" s="84">
+        <v>107</v>
+      </c>
+      <c r="E19" t="s" s="84">
         <v>108</v>
-      </c>
-      <c r="E19" t="s" s="84">
-        <v>109</v>
       </c>
       <c r="F19" s="111">
         <v>3640</v>
@@ -9327,10 +9324,10 @@
         <v>1840</v>
       </c>
       <c r="J19" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K19" t="s" s="84">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L19" s="111">
         <v>120</v>
@@ -9345,7 +9342,7 @@
       <c r="O19" s="101"/>
       <c r="P19" s="57"/>
       <c r="Q19" t="s" s="84">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="R19" t="s" s="84">
         <v>214</v>
@@ -9354,13 +9351,13 @@
         <v>215</v>
       </c>
       <c r="T19" t="s" s="114">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U19" t="s" s="115">
         <v>187</v>
       </c>
       <c r="V19" t="s" s="84">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="W19" s="116"/>
       <c r="X19" s="62"/>
@@ -9398,10 +9395,10 @@
         <v>45900</v>
       </c>
       <c r="D20" t="s" s="84">
+        <v>123</v>
+      </c>
+      <c r="E20" t="s" s="84">
         <v>124</v>
-      </c>
-      <c r="E20" t="s" s="84">
-        <v>125</v>
       </c>
       <c r="F20" s="111">
         <v>3615</v>
@@ -9417,10 +9414,10 @@
         <v>1930</v>
       </c>
       <c r="J20" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K20" t="s" s="84">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L20" s="111">
         <v>125</v>
@@ -9444,13 +9441,13 @@
         <v>223</v>
       </c>
       <c r="T20" t="s" s="114">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="U20" t="s" s="115">
         <v>197</v>
       </c>
       <c r="V20" t="s" s="84">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W20" s="116"/>
       <c r="X20" s="62"/>
@@ -9491,7 +9488,7 @@
         <v>229</v>
       </c>
       <c r="E21" t="s" s="84">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F21" s="111">
         <v>3510</v>
@@ -9507,10 +9504,10 @@
         <v>2085</v>
       </c>
       <c r="J21" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K21" t="s" s="84">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L21" s="111">
         <v>27</v>
@@ -9525,7 +9522,7 @@
       <c r="O21" s="101"/>
       <c r="P21" s="57"/>
       <c r="Q21" t="s" s="84">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="R21" t="s" s="84">
         <v>230</v>
@@ -9540,7 +9537,7 @@
         <v>233</v>
       </c>
       <c r="V21" t="s" s="84">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="W21" s="116"/>
       <c r="X21" s="62"/>
@@ -9560,7 +9557,7 @@
         <v>238</v>
       </c>
       <c r="AD21" t="s" s="84">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AE21" s="117"/>
       <c r="AF21" s="48"/>
@@ -9599,10 +9596,10 @@
         <v>2085</v>
       </c>
       <c r="J22" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K22" t="s" s="84">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L22" s="111">
         <v>115</v>
@@ -9632,7 +9629,7 @@
         <v>243</v>
       </c>
       <c r="V22" t="s" s="84">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W22" s="116"/>
       <c r="X22" s="62"/>
@@ -9691,10 +9688,10 @@
         <v>2085</v>
       </c>
       <c r="J23" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K23" t="s" s="84">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L23" s="111">
         <v>120</v>
@@ -9724,7 +9721,7 @@
         <v>243</v>
       </c>
       <c r="V23" t="s" s="84">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W23" s="116"/>
       <c r="X23" s="62"/>
@@ -9783,10 +9780,10 @@
         <v>2085</v>
       </c>
       <c r="J24" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K24" t="s" s="84">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L24" s="111">
         <v>125</v>
@@ -9816,7 +9813,7 @@
         <v>265</v>
       </c>
       <c r="V24" t="s" s="84">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W24" s="116"/>
       <c r="X24" s="122"/>
@@ -9836,7 +9833,7 @@
         <v>270</v>
       </c>
       <c r="AD24" t="s" s="84">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AE24" s="117"/>
       <c r="AF24" s="48"/>
@@ -10020,7 +10017,7 @@
     <row r="6" ht="96" customHeight="1">
       <c r="A6" s="71"/>
       <c r="B6" t="s" s="72">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s" s="73">
         <v>273</v>
@@ -10059,13 +10056,13 @@
         <v>283</v>
       </c>
       <c r="B7" t="s" s="84">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s" s="91">
         <v>284</v>
       </c>
       <c r="D7" t="s" s="87">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7" t="s" s="87">
         <v>285</v>
@@ -10095,7 +10092,7 @@
     </row>
     <row r="8" ht="96" customHeight="1">
       <c r="A8" t="s" s="94">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="95" cm="1">
         <f t="array" ref="B8">IF(COUNTA(C8:H8)=0,"",9992+ROW())</f>
@@ -10105,7 +10102,7 @@
         <v>45806</v>
       </c>
       <c r="D8" t="s" s="97">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s" s="97">
         <v>293</v>
@@ -10118,7 +10115,7 @@
       </c>
       <c r="H8" s="107"/>
       <c r="I8" t="s" s="97">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J8" s="98">
         <v>5</v>
@@ -10144,10 +10141,10 @@
         <v>297</v>
       </c>
       <c r="E9" t="s" s="84">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F9" t="s" s="84">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G9" s="110">
         <v>45823</v>
@@ -10156,13 +10153,13 @@
         <v>298</v>
       </c>
       <c r="I9" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J9" s="111">
         <v>505</v>
       </c>
       <c r="K9" t="s" s="84">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L9" t="s" s="84">
         <v>299</v>
@@ -10182,7 +10179,7 @@
         <v>300</v>
       </c>
       <c r="E10" t="s" s="84">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F10" t="s" s="84">
         <v>301</v>
@@ -10194,13 +10191,13 @@
         <v>302</v>
       </c>
       <c r="I10" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J10" s="111">
         <v>140</v>
       </c>
       <c r="K10" t="s" s="84">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L10" t="s" s="84">
         <v>303</v>
@@ -10220,7 +10217,7 @@
         <v>304</v>
       </c>
       <c r="E11" t="s" s="84">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F11" t="s" s="84">
         <v>305</v>
@@ -10232,13 +10229,13 @@
         <v>306</v>
       </c>
       <c r="I11" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J11" s="111">
         <v>75</v>
       </c>
       <c r="K11" t="s" s="84">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L11" t="s" s="84">
         <v>307</v>
@@ -10258,10 +10255,10 @@
         <v>300</v>
       </c>
       <c r="E12" t="s" s="84">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F12" t="s" s="84">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G12" s="110">
         <v>45824</v>
@@ -10270,13 +10267,13 @@
         <v>308</v>
       </c>
       <c r="I12" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J12" s="111">
         <v>515</v>
       </c>
       <c r="K12" t="s" s="84">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L12" t="s" s="84">
         <v>309</v>
@@ -10308,7 +10305,7 @@
         <v>302</v>
       </c>
       <c r="I13" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J13" s="111">
         <v>140</v>
@@ -10346,7 +10343,7 @@
         <v>306</v>
       </c>
       <c r="I14" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J14" s="111">
         <v>75</v>
@@ -10375,7 +10372,7 @@
         <v>180</v>
       </c>
       <c r="F15" t="s" s="84">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G15" s="110">
         <v>45825</v>
@@ -10384,13 +10381,13 @@
         <v>315</v>
       </c>
       <c r="I15" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J15" s="111">
         <v>525</v>
       </c>
       <c r="K15" t="s" s="84">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L15" t="s" s="84">
         <v>316</v>
@@ -10422,7 +10419,7 @@
         <v>302</v>
       </c>
       <c r="I16" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J16" s="111">
         <v>140</v>
@@ -10460,7 +10457,7 @@
         <v>306</v>
       </c>
       <c r="I17" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J17" s="111">
         <v>75</v>
@@ -10489,7 +10486,7 @@
         <v>211</v>
       </c>
       <c r="F18" t="s" s="84">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G18" s="110">
         <v>45826</v>
@@ -10498,7 +10495,7 @@
         <v>320</v>
       </c>
       <c r="I18" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J18" s="111">
         <v>535</v>
@@ -10536,13 +10533,13 @@
         <v>306</v>
       </c>
       <c r="I19" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J19" s="111">
         <v>140</v>
       </c>
       <c r="K19" t="s" s="84">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L19" t="s" s="84">
         <v>322</v>
@@ -10574,7 +10571,7 @@
         <v>320</v>
       </c>
       <c r="I20" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J20" s="111">
         <v>75</v>
@@ -10612,13 +10609,13 @@
         <v>325</v>
       </c>
       <c r="I21" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J21" s="111">
         <v>25</v>
       </c>
       <c r="K21" t="s" s="84">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L21" t="s" s="84">
         <v>326</v>
@@ -10650,7 +10647,7 @@
         <v>302</v>
       </c>
       <c r="I22" t="s" s="84">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J22" s="111">
         <v>20</v>
@@ -10688,7 +10685,7 @@
         <v>306</v>
       </c>
       <c r="I23" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J23" s="111">
         <v>15</v>
@@ -10726,7 +10723,7 @@
         <v>298</v>
       </c>
       <c r="I24" t="s" s="84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J24" s="111">
         <v>10</v>
@@ -10892,16 +10889,16 @@
     <row r="6" ht="96" customHeight="1">
       <c r="A6" s="71"/>
       <c r="B6" t="s" s="72">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s" s="72">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s" s="73">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s" s="73">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s" s="73">
         <v>273</v>
@@ -10945,22 +10942,22 @@
         <v>342</v>
       </c>
       <c r="B7" t="s" s="84">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s" s="84">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s" s="84">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s" s="84">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s" s="91">
         <v>284</v>
       </c>
       <c r="G7" t="s" s="129">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H7" t="s" s="135">
         <v>343</v>
@@ -10984,7 +10981,7 @@
         <v>349</v>
       </c>
       <c r="O7" t="s" s="87">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P7" s="137"/>
       <c r="Q7" s="137"/>
@@ -10995,26 +10992,26 @@
     </row>
     <row r="8" ht="96" customHeight="1">
       <c r="A8" t="s" s="94">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="95" cm="1">
         <f t="array" ref="B8">IF(COUNTA(F8:H8)=0,"",9992+ROW())</f>
         <v>10000</v>
       </c>
       <c r="C8" t="s" s="138">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" t="s" s="97">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" t="s" s="97">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F8" s="96">
         <v>45806</v>
       </c>
       <c r="G8" t="s" s="97">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H8" s="100">
         <v>50</v>
@@ -11058,7 +11055,7 @@
         <v>354</v>
       </c>
       <c r="E9" t="s" s="84">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F9" s="110">
         <v>45806</v>
@@ -11073,22 +11070,22 @@
         <v>355</v>
       </c>
       <c r="J9" t="s" s="84">
+        <v>95</v>
+      </c>
+      <c r="K9" t="s" s="84">
         <v>96</v>
       </c>
-      <c r="K9" t="s" s="84">
+      <c r="L9" t="s" s="84">
         <v>97</v>
       </c>
-      <c r="L9" t="s" s="84">
+      <c r="M9" t="s" s="114">
         <v>98</v>
       </c>
-      <c r="M9" t="s" s="114">
+      <c r="N9" t="s" s="115">
         <v>99</v>
       </c>
-      <c r="N9" t="s" s="115">
-        <v>100</v>
-      </c>
       <c r="O9" t="s" s="84">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P9" s="134"/>
       <c r="Q9" s="134"/>
@@ -11104,13 +11101,13 @@
         <v>10002</v>
       </c>
       <c r="C10" t="s" s="84">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" t="s" s="84">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E10" t="s" s="84">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F10" s="110">
         <v>45807</v>
@@ -11125,22 +11122,22 @@
         <v>356</v>
       </c>
       <c r="J10" t="s" s="84">
+        <v>111</v>
+      </c>
+      <c r="K10" t="s" s="84">
         <v>112</v>
       </c>
-      <c r="K10" t="s" s="84">
+      <c r="L10" t="s" s="84">
         <v>113</v>
       </c>
-      <c r="L10" t="s" s="84">
+      <c r="M10" t="s" s="114">
         <v>114</v>
       </c>
-      <c r="M10" t="s" s="114">
+      <c r="N10" t="s" s="115">
         <v>115</v>
       </c>
-      <c r="N10" t="s" s="115">
-        <v>116</v>
-      </c>
       <c r="O10" t="s" s="84">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P10" s="134"/>
       <c r="Q10" s="134"/>
@@ -11159,10 +11156,10 @@
         <v>357</v>
       </c>
       <c r="D11" t="s" s="84">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E11" t="s" s="84">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F11" s="110">
         <v>45808</v>
@@ -11177,22 +11174,22 @@
         <v>350</v>
       </c>
       <c r="J11" t="s" s="84">
+        <v>126</v>
+      </c>
+      <c r="K11" t="s" s="84">
         <v>127</v>
       </c>
-      <c r="K11" t="s" s="84">
+      <c r="L11" t="s" s="84">
         <v>128</v>
       </c>
-      <c r="L11" t="s" s="84">
+      <c r="M11" t="s" s="114">
         <v>129</v>
       </c>
-      <c r="M11" t="s" s="114">
+      <c r="N11" t="s" s="115">
         <v>130</v>
       </c>
-      <c r="N11" t="s" s="115">
-        <v>131</v>
-      </c>
       <c r="O11" t="s" s="84">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P11" s="134"/>
       <c r="Q11" s="134"/>
@@ -11211,10 +11208,10 @@
         <v>358</v>
       </c>
       <c r="D12" t="s" s="84">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E12" t="s" s="84">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F12" s="110">
         <v>45807</v>
@@ -11229,22 +11226,22 @@
         <v>350</v>
       </c>
       <c r="J12" t="s" s="84">
+        <v>141</v>
+      </c>
+      <c r="K12" t="s" s="84">
         <v>142</v>
       </c>
-      <c r="K12" t="s" s="84">
+      <c r="L12" t="s" s="84">
         <v>143</v>
       </c>
-      <c r="L12" t="s" s="84">
+      <c r="M12" t="s" s="114">
         <v>144</v>
       </c>
-      <c r="M12" t="s" s="114">
-        <v>145</v>
-      </c>
       <c r="N12" t="s" s="115">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O12" t="s" s="84">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P12" s="134"/>
       <c r="Q12" s="134"/>
@@ -11263,10 +11260,10 @@
         <v>359</v>
       </c>
       <c r="D13" t="s" s="84">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E13" t="s" s="84">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F13" s="110">
         <v>45808</v>
@@ -11290,7 +11287,7 @@
         <v>155</v>
       </c>
       <c r="M13" t="s" s="114">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N13" t="s" s="115">
         <v>156</v>
@@ -11315,10 +11312,10 @@
         <v>360</v>
       </c>
       <c r="D14" t="s" s="84">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E14" t="s" s="84">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F14" s="110">
         <v>45809</v>
@@ -11342,7 +11339,7 @@
         <v>165</v>
       </c>
       <c r="M14" t="s" s="114">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N14" t="s" s="115">
         <v>166</v>
@@ -11367,7 +11364,7 @@
         <v>361</v>
       </c>
       <c r="D15" t="s" s="84">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E15" t="s" s="84">
         <v>173</v>
@@ -11385,7 +11382,7 @@
         <v>350</v>
       </c>
       <c r="J15" t="s" s="84">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K15" t="s" s="84">
         <v>175</v>
@@ -11394,7 +11391,7 @@
         <v>176</v>
       </c>
       <c r="M15" t="s" s="114">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N15" t="s" s="115">
         <v>177</v>
@@ -11422,7 +11419,7 @@
         <v>174</v>
       </c>
       <c r="E16" t="s" s="84">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F16" s="110">
         <v>45809</v>
@@ -11471,10 +11468,10 @@
         <v>363</v>
       </c>
       <c r="D17" t="s" s="84">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E17" t="s" s="84">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F17" s="110">
         <v>45810</v>
@@ -11504,7 +11501,7 @@
         <v>197</v>
       </c>
       <c r="O17" t="s" s="84">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P17" s="134"/>
       <c r="Q17" s="134"/>
@@ -11523,7 +11520,7 @@
         <v>364</v>
       </c>
       <c r="D18" t="s" s="84">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E18" t="s" s="84">
         <v>203</v>
@@ -11556,7 +11553,7 @@
         <v>177</v>
       </c>
       <c r="O18" t="s" s="84">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P18" s="134"/>
       <c r="Q18" s="134"/>
@@ -11578,7 +11575,7 @@
         <v>204</v>
       </c>
       <c r="E19" t="s" s="84">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F19" s="110">
         <v>45810</v>
@@ -11593,7 +11590,7 @@
         <v>350</v>
       </c>
       <c r="J19" t="s" s="84">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K19" t="s" s="84">
         <v>214</v>
@@ -11602,7 +11599,7 @@
         <v>215</v>
       </c>
       <c r="M19" t="s" s="114">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N19" t="s" s="115">
         <v>187</v>
@@ -11625,10 +11622,10 @@
         <v>366</v>
       </c>
       <c r="D20" t="s" s="84">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E20" t="s" s="84">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F20" s="110">
         <v>45811</v>
@@ -11652,7 +11649,7 @@
         <v>223</v>
       </c>
       <c r="M20" t="s" s="114">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N20" t="s" s="115">
         <v>197</v>
@@ -11675,7 +11672,7 @@
         <v>367</v>
       </c>
       <c r="D21" t="s" s="84">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E21" t="s" s="84">
         <v>229</v>
@@ -11693,7 +11690,7 @@
         <v>356</v>
       </c>
       <c r="J21" t="s" s="84">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K21" t="s" s="84">
         <v>230</v>
@@ -11708,7 +11705,7 @@
         <v>233</v>
       </c>
       <c r="O21" t="s" s="84">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P21" s="134"/>
       <c r="Q21" s="134"/>
@@ -11727,7 +11724,7 @@
         <v>368</v>
       </c>
       <c r="D22" t="s" s="84">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E22" t="s" s="84">
         <v>173</v>
@@ -11864,7 +11861,7 @@
         <v>265</v>
       </c>
       <c r="O24" t="s" s="84">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P24" s="140"/>
       <c r="Q24" s="140"/>
@@ -11938,7 +11935,7 @@
   <sheetData>
     <row r="1" s="143" customFormat="1" ht="29" customHeight="1">
       <c r="A1" t="s" s="144">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s" s="144">
         <v>371</v>
@@ -12130,7 +12127,7 @@
         <v>433</v>
       </c>
       <c r="BM1" t="s" s="144">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BN1" t="s" s="144">
         <v>434</v>
@@ -12166,7 +12163,7 @@
         <v>249</v>
       </c>
       <c r="BY1" t="s" s="144">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BZ1" t="s" s="144">
         <v>444</v>
@@ -14568,7 +14565,7 @@
     </row>
     <row r="2" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A2" t="s" s="144">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s" s="144">
         <v>1196</v>
@@ -14619,10 +14616,10 @@
         <v>1211</v>
       </c>
       <c r="R2" t="s" s="144">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S2" t="s" s="144">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T2" t="s" s="144">
         <v>1212</v>
@@ -14637,7 +14634,7 @@
         <v>1214</v>
       </c>
       <c r="X2" t="s" s="144">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Y2" t="s" s="144">
         <v>1215</v>
@@ -14655,7 +14652,7 @@
         <v>204</v>
       </c>
       <c r="AD2" t="s" s="144">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AE2" t="s" s="144">
         <v>174</v>
@@ -14744,7 +14741,7 @@
     </row>
     <row r="15" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A15" t="s" s="144">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s" s="144">
         <v>1237</v>
@@ -14752,7 +14749,7 @@
     </row>
     <row r="16" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A16" t="s" s="144">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s" s="144">
         <v>1238</v>
@@ -14760,7 +14757,7 @@
     </row>
     <row r="17" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A17" t="s" s="144">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s" s="144">
         <v>1239</v>
@@ -14768,7 +14765,7 @@
     </row>
     <row r="18" s="143" customFormat="1" ht="42" customHeight="1">
       <c r="A18" t="s" s="156">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s" s="144">
         <v>1240</v>
@@ -14776,7 +14773,7 @@
     </row>
     <row r="19" s="143" customFormat="1" ht="29" customHeight="1">
       <c r="A19" t="s" s="156">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s" s="144">
         <v>1241</v>
@@ -14784,7 +14781,7 @@
     </row>
     <row r="20" s="143" customFormat="1" ht="29" customHeight="1">
       <c r="A20" t="s" s="156">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s" s="144">
         <v>1242</v>
@@ -14792,7 +14789,7 @@
     </row>
     <row r="21" s="143" customFormat="1" ht="42" customHeight="1">
       <c r="A21" t="s" s="156">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s" s="144">
         <v>1243</v>
@@ -14800,7 +14797,7 @@
     </row>
     <row r="22" s="143" customFormat="1" ht="29" customHeight="1">
       <c r="A22" t="s" s="156">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s" s="144">
         <v>1244</v>
@@ -14808,7 +14805,7 @@
     </row>
     <row r="23" s="143" customFormat="1" ht="55" customHeight="1">
       <c r="A23" t="s" s="156">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s" s="144">
         <v>1245</v>
@@ -14816,7 +14813,7 @@
     </row>
     <row r="24" s="143" customFormat="1" ht="42" customHeight="1">
       <c r="A24" t="s" s="156">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s" s="144">
         <v>1246</v>
@@ -14824,7 +14821,7 @@
     </row>
     <row r="25" s="143" customFormat="1" ht="42" customHeight="1">
       <c r="A25" t="s" s="156">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s" s="144">
         <v>1247</v>
@@ -14832,7 +14829,7 @@
     </row>
     <row r="26" s="143" customFormat="1" ht="29" customHeight="1">
       <c r="A26" t="s" s="156">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s" s="144">
         <v>1248</v>
@@ -14840,7 +14837,7 @@
     </row>
     <row r="27" s="143" customFormat="1" ht="42" customHeight="1">
       <c r="A27" t="s" s="156">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s" s="144">
         <v>1249</v>
@@ -14848,7 +14845,7 @@
     </row>
     <row r="30" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A30" t="s" s="144">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s" s="144">
         <v>1250</v>
@@ -14856,7 +14853,7 @@
     </row>
     <row r="31" s="143" customFormat="1" ht="29" customHeight="1">
       <c r="A31" t="s" s="156">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s" s="144">
         <v>1251</v>
@@ -14864,7 +14861,7 @@
     </row>
     <row r="32" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A32" t="s" s="144">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s" s="144">
         <v>1252</v>
@@ -14872,7 +14869,7 @@
     </row>
     <row r="33" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A33" t="s" s="144">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s" s="144">
         <v>1253</v>
@@ -14880,7 +14877,7 @@
     </row>
     <row r="34" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A34" t="s" s="144">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" t="s" s="144">
         <v>1254</v>
@@ -14888,7 +14885,7 @@
     </row>
     <row r="35" s="143" customFormat="1" ht="55" customHeight="1">
       <c r="A35" t="s" s="156">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s" s="144">
         <v>1255</v>
@@ -14902,7 +14899,7 @@
     </row>
     <row r="39" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A39" t="s" s="144">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B39" t="s" s="144">
         <v>1237</v>
@@ -14990,7 +14987,7 @@
     </row>
     <row r="52" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A52" t="s" s="144">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B52" t="s" s="144">
         <v>1237</v>
@@ -14998,7 +14995,7 @@
     </row>
     <row r="53" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A53" t="s" s="144">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B53" t="s" s="144">
         <v>1266</v>
@@ -15006,7 +15003,7 @@
     </row>
     <row r="54" s="143" customFormat="1" ht="42" customHeight="1">
       <c r="A54" t="s" s="156">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B54" t="s" s="144">
         <v>1240</v>
@@ -15014,7 +15011,7 @@
     </row>
     <row r="55" s="143" customFormat="1" ht="17" customHeight="1">
       <c r="A55" t="s" s="144">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B55" t="s" s="144">
         <v>1239</v>
@@ -15097,7 +15094,7 @@
         <v>341</v>
       </c>
       <c r="B65" t="s" s="144">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>